<commit_message>
added dummy kill and edited planning
</commit_message>
<xml_diff>
--- a/PLANNING/Task Planning.xlsx
+++ b/PLANNING/Task Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoftwareProjects\Unity\Band-Battle\PLANNING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECEFF4C-BF09-40AB-ADB5-8D6CF4BF04FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83BF412C-ADB8-4D87-8688-FCCF830EFF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{70D4C62D-D84E-421C-8B35-459A60CD8044}"/>
   </bookViews>
@@ -856,7 +856,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
@@ -934,10 +934,39 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -955,39 +984,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="30" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -1316,7 +1312,7 @@
       <pane xSplit="4" ySplit="10" topLeftCell="E11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
+      <selection pane="bottomRight" activeCell="AK16" sqref="AK16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1329,69 +1325,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="F1" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="52"/>
+      <c r="F1" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="61"/>
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="F2" s="32"/>
-      <c r="G2" s="46" t="s">
+      <c r="G2" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="47"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="66"/>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="F3" s="29"/>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="46"/>
-      <c r="N3" s="47"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="65"/>
+      <c r="L3" s="65"/>
+      <c r="M3" s="65"/>
+      <c r="N3" s="66"/>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="F4" s="31"/>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="46"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="47"/>
+      <c r="H4" s="65"/>
+      <c r="I4" s="65"/>
+      <c r="J4" s="65"/>
+      <c r="K4" s="65"/>
+      <c r="L4" s="65"/>
+      <c r="M4" s="65"/>
+      <c r="N4" s="66"/>
     </row>
     <row r="5" spans="1:60" ht="14.55" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F5" s="30"/>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
-      <c r="N5" s="49"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="67"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="68"/>
     </row>
     <row r="7" spans="1:60" ht="21.6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="11"/>
@@ -1400,78 +1396,78 @@
       <c r="D7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="44" t="s">
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="43"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="43"/>
-      <c r="P7" s="43"/>
-      <c r="Q7" s="43"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="44" t="s">
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="64"/>
+      <c r="S7" s="62" t="s">
         <v>6</v>
       </c>
-      <c r="T7" s="43"/>
-      <c r="U7" s="43"/>
-      <c r="V7" s="43"/>
-      <c r="W7" s="43"/>
-      <c r="X7" s="43"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="44" t="s">
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="64"/>
+      <c r="Z7" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="AA7" s="43"/>
-      <c r="AB7" s="43"/>
-      <c r="AC7" s="43"/>
-      <c r="AD7" s="43"/>
-      <c r="AE7" s="43"/>
-      <c r="AF7" s="45"/>
-      <c r="AG7" s="44" t="s">
+      <c r="AA7" s="63"/>
+      <c r="AB7" s="63"/>
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="63"/>
+      <c r="AE7" s="63"/>
+      <c r="AF7" s="64"/>
+      <c r="AG7" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="AH7" s="43"/>
-      <c r="AI7" s="43"/>
-      <c r="AJ7" s="43"/>
-      <c r="AK7" s="43"/>
-      <c r="AL7" s="43"/>
-      <c r="AM7" s="45"/>
-      <c r="AN7" s="44" t="s">
+      <c r="AH7" s="63"/>
+      <c r="AI7" s="63"/>
+      <c r="AJ7" s="63"/>
+      <c r="AK7" s="63"/>
+      <c r="AL7" s="63"/>
+      <c r="AM7" s="64"/>
+      <c r="AN7" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="AO7" s="43"/>
-      <c r="AP7" s="43"/>
-      <c r="AQ7" s="43"/>
-      <c r="AR7" s="43"/>
-      <c r="AS7" s="43"/>
-      <c r="AT7" s="45"/>
-      <c r="AU7" s="44" t="s">
+      <c r="AO7" s="63"/>
+      <c r="AP7" s="63"/>
+      <c r="AQ7" s="63"/>
+      <c r="AR7" s="63"/>
+      <c r="AS7" s="63"/>
+      <c r="AT7" s="64"/>
+      <c r="AU7" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AV7" s="43"/>
-      <c r="AW7" s="43"/>
-      <c r="AX7" s="43"/>
-      <c r="AY7" s="43"/>
-      <c r="AZ7" s="43"/>
-      <c r="BA7" s="45"/>
-      <c r="BB7" s="44" t="s">
+      <c r="AV7" s="63"/>
+      <c r="AW7" s="63"/>
+      <c r="AX7" s="63"/>
+      <c r="AY7" s="63"/>
+      <c r="AZ7" s="63"/>
+      <c r="BA7" s="64"/>
+      <c r="BB7" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="BC7" s="43"/>
-      <c r="BD7" s="43"/>
-      <c r="BE7" s="43"/>
-      <c r="BF7" s="43"/>
-      <c r="BG7" s="43"/>
-      <c r="BH7" s="45"/>
+      <c r="BC7" s="63"/>
+      <c r="BD7" s="63"/>
+      <c r="BE7" s="63"/>
+      <c r="BF7" s="63"/>
+      <c r="BG7" s="63"/>
+      <c r="BH7" s="64"/>
     </row>
     <row r="8" spans="1:60" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14"/>
@@ -1904,7 +1900,7 @@
       <c r="BH10" s="7"/>
     </row>
     <row r="11" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="51" t="s">
         <v>29</v>
       </c>
       <c r="B11" s="25" t="s">
@@ -1916,62 +1912,61 @@
       <c r="D11" s="33">
         <v>0</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="57"/>
-      <c r="M11" s="55"/>
-      <c r="N11" s="55"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="55"/>
-      <c r="Q11" s="55"/>
-      <c r="R11" s="56"/>
-      <c r="S11" s="57"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="55"/>
-      <c r="V11" s="55"/>
-      <c r="W11" s="55"/>
-      <c r="X11" s="55"/>
-      <c r="Y11" s="56"/>
-      <c r="Z11" s="57"/>
-      <c r="AA11" s="55"/>
-      <c r="AB11" s="55"/>
-      <c r="AC11" s="55"/>
-      <c r="AD11" s="55"/>
-      <c r="AE11" s="55"/>
-      <c r="AF11" s="56"/>
-      <c r="AG11" s="57"/>
-      <c r="AH11" s="55"/>
-      <c r="AI11" s="55"/>
-      <c r="AJ11" s="55"/>
-      <c r="AK11" s="55"/>
-      <c r="AL11" s="55"/>
-      <c r="AM11" s="56"/>
-      <c r="AN11" s="57"/>
-      <c r="AO11" s="55"/>
-      <c r="AP11" s="55"/>
-      <c r="AQ11" s="55"/>
-      <c r="AR11" s="55"/>
-      <c r="AS11" s="55"/>
-      <c r="AT11" s="72"/>
-      <c r="AU11" s="57"/>
-      <c r="AV11" s="55"/>
-      <c r="AW11" s="55"/>
-      <c r="AX11" s="55"/>
-      <c r="AY11" s="55"/>
-      <c r="AZ11" s="55"/>
-      <c r="BA11" s="56"/>
-      <c r="BB11" s="57"/>
-      <c r="BC11" s="55"/>
-      <c r="BD11" s="55"/>
-      <c r="BE11" s="55"/>
-      <c r="BF11" s="55"/>
-      <c r="BG11" s="55"/>
-      <c r="BH11" s="56"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="45"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="46"/>
+      <c r="L11" s="47"/>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="46"/>
+      <c r="S11" s="47"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="46"/>
+      <c r="Z11" s="47"/>
+      <c r="AA11" s="45"/>
+      <c r="AB11" s="45"/>
+      <c r="AC11" s="45"/>
+      <c r="AD11" s="45"/>
+      <c r="AE11" s="45"/>
+      <c r="AF11" s="46"/>
+      <c r="AG11" s="47"/>
+      <c r="AH11" s="45"/>
+      <c r="AI11" s="45"/>
+      <c r="AJ11" s="45"/>
+      <c r="AK11" s="45"/>
+      <c r="AL11" s="45"/>
+      <c r="AM11" s="46"/>
+      <c r="AN11" s="47"/>
+      <c r="AO11" s="45"/>
+      <c r="AP11" s="45"/>
+      <c r="AQ11" s="45"/>
+      <c r="AR11" s="45"/>
+      <c r="AS11" s="45"/>
+      <c r="AT11" s="58"/>
+      <c r="AU11" s="47"/>
+      <c r="AV11" s="45"/>
+      <c r="AW11" s="45"/>
+      <c r="AX11" s="45"/>
+      <c r="AY11" s="45"/>
+      <c r="AZ11" s="45"/>
+      <c r="BA11" s="46"/>
+      <c r="BB11" s="47"/>
+      <c r="BC11" s="57"/>
+      <c r="BD11" s="45"/>
+      <c r="BE11" s="45"/>
+      <c r="BF11" s="45"/>
+      <c r="BG11" s="45"/>
+      <c r="BH11" s="46"/>
     </row>
     <row r="12" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="25" t="s">
@@ -1982,62 +1977,32 @@
       <c r="D12" s="33">
         <v>0</v>
       </c>
-      <c r="E12" s="63"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="70"/>
-      <c r="K12" s="70"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="60"/>
-      <c r="T12" s="61"/>
-      <c r="U12" s="61"/>
-      <c r="V12" s="61"/>
-      <c r="W12" s="61"/>
-      <c r="X12" s="61"/>
-      <c r="Y12" s="68"/>
-      <c r="Z12" s="60"/>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="61"/>
-      <c r="AC12" s="61"/>
-      <c r="AD12" s="61"/>
-      <c r="AE12" s="61"/>
-      <c r="AF12" s="59"/>
-      <c r="AG12" s="60"/>
-      <c r="AH12" s="61"/>
-      <c r="AI12" s="61"/>
-      <c r="AJ12" s="61"/>
-      <c r="AK12" s="61"/>
-      <c r="AL12" s="61"/>
-      <c r="AM12" s="59"/>
-      <c r="AN12" s="60"/>
-      <c r="AO12" s="61"/>
-      <c r="AP12" s="61"/>
-      <c r="AQ12" s="61"/>
-      <c r="AR12" s="61"/>
-      <c r="AS12" s="61"/>
-      <c r="AT12" s="72"/>
-      <c r="AU12" s="60"/>
-      <c r="AV12" s="61"/>
-      <c r="AW12" s="61"/>
-      <c r="AX12" s="61"/>
-      <c r="AY12" s="61"/>
-      <c r="AZ12" s="61"/>
-      <c r="BA12" s="59"/>
-      <c r="BB12" s="60"/>
-      <c r="BC12" s="61"/>
-      <c r="BD12" s="61"/>
-      <c r="BE12" s="61"/>
-      <c r="BF12" s="61"/>
-      <c r="BG12" s="61"/>
-      <c r="BH12" s="59"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="50"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="55"/>
+      <c r="O12" s="55"/>
+      <c r="P12" s="55"/>
+      <c r="Q12" s="55"/>
+      <c r="R12" s="54"/>
+      <c r="S12" s="35"/>
+      <c r="Y12" s="54"/>
+      <c r="Z12" s="35"/>
+      <c r="AF12" s="36"/>
+      <c r="AG12" s="35"/>
+      <c r="AM12" s="36"/>
+      <c r="AN12" s="35"/>
+      <c r="AT12" s="58"/>
+      <c r="AU12" s="35"/>
+      <c r="BA12" s="36"/>
+      <c r="BB12" s="35"/>
+      <c r="BC12" s="57"/>
+      <c r="BH12" s="36"/>
     </row>
     <row r="13" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="25" t="s">
@@ -2050,62 +2015,24 @@
       <c r="D13" s="33">
         <v>0</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="59"/>
-      <c r="L13" s="60"/>
-      <c r="M13" s="61"/>
-      <c r="N13" s="61"/>
-      <c r="O13" s="61"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="61"/>
-      <c r="R13" s="59"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="61"/>
-      <c r="U13" s="61"/>
-      <c r="V13" s="61"/>
-      <c r="W13" s="61"/>
-      <c r="X13" s="61"/>
-      <c r="Y13" s="59"/>
-      <c r="Z13" s="60"/>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="61"/>
-      <c r="AC13" s="61"/>
-      <c r="AD13" s="61"/>
-      <c r="AE13" s="61"/>
-      <c r="AF13" s="59"/>
-      <c r="AG13" s="60"/>
-      <c r="AH13" s="61"/>
-      <c r="AI13" s="61"/>
-      <c r="AJ13" s="61"/>
-      <c r="AK13" s="61"/>
-      <c r="AL13" s="61"/>
-      <c r="AM13" s="68"/>
-      <c r="AN13" s="60"/>
-      <c r="AO13" s="61"/>
-      <c r="AP13" s="61"/>
-      <c r="AQ13" s="61"/>
-      <c r="AR13" s="61"/>
-      <c r="AS13" s="61"/>
-      <c r="AT13" s="72"/>
-      <c r="AU13" s="60"/>
-      <c r="AV13" s="61"/>
-      <c r="AW13" s="61"/>
-      <c r="AX13" s="61"/>
-      <c r="AY13" s="61"/>
-      <c r="AZ13" s="61"/>
-      <c r="BA13" s="59"/>
-      <c r="BB13" s="60"/>
-      <c r="BC13" s="61"/>
-      <c r="BD13" s="61"/>
-      <c r="BE13" s="61"/>
-      <c r="BF13" s="61"/>
-      <c r="BG13" s="61"/>
-      <c r="BH13" s="59"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="50"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="35"/>
+      <c r="R13" s="36"/>
+      <c r="S13" s="35"/>
+      <c r="Y13" s="36"/>
+      <c r="Z13" s="35"/>
+      <c r="AF13" s="36"/>
+      <c r="AG13" s="35"/>
+      <c r="AM13" s="54"/>
+      <c r="AN13" s="35"/>
+      <c r="AT13" s="58"/>
+      <c r="AU13" s="35"/>
+      <c r="BA13" s="36"/>
+      <c r="BB13" s="35"/>
+      <c r="BC13" s="57"/>
+      <c r="BH13" s="36"/>
     </row>
     <row r="14" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="25" t="s">
@@ -2118,65 +2045,27 @@
       <c r="D14" s="33">
         <v>0</v>
       </c>
-      <c r="E14" s="63"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="59"/>
-      <c r="L14" s="60"/>
-      <c r="M14" s="61"/>
-      <c r="N14" s="61"/>
-      <c r="O14" s="61"/>
-      <c r="P14" s="61"/>
-      <c r="Q14" s="61"/>
-      <c r="R14" s="59"/>
-      <c r="S14" s="60"/>
-      <c r="T14" s="61"/>
-      <c r="U14" s="61"/>
-      <c r="V14" s="61"/>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
-      <c r="Y14" s="59"/>
-      <c r="Z14" s="60"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="61"/>
-      <c r="AC14" s="61"/>
-      <c r="AD14" s="61"/>
-      <c r="AE14" s="61"/>
-      <c r="AF14" s="59"/>
-      <c r="AG14" s="60"/>
-      <c r="AH14" s="61"/>
-      <c r="AI14" s="61"/>
-      <c r="AJ14" s="61"/>
-      <c r="AK14" s="61"/>
-      <c r="AL14" s="61"/>
-      <c r="AM14" s="68"/>
-      <c r="AN14" s="60"/>
-      <c r="AO14" s="61"/>
-      <c r="AP14" s="61"/>
-      <c r="AQ14" s="61"/>
-      <c r="AR14" s="61"/>
-      <c r="AS14" s="61"/>
-      <c r="AT14" s="72"/>
-      <c r="AU14" s="60"/>
-      <c r="AV14" s="61"/>
-      <c r="AW14" s="61"/>
-      <c r="AX14" s="61"/>
-      <c r="AY14" s="61"/>
-      <c r="AZ14" s="61"/>
-      <c r="BA14" s="59"/>
-      <c r="BB14" s="60"/>
-      <c r="BC14" s="61"/>
-      <c r="BD14" s="61"/>
-      <c r="BE14" s="61"/>
-      <c r="BF14" s="61"/>
-      <c r="BG14" s="61"/>
-      <c r="BH14" s="59"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="50"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="35"/>
+      <c r="R14" s="36"/>
+      <c r="S14" s="35"/>
+      <c r="Y14" s="36"/>
+      <c r="Z14" s="35"/>
+      <c r="AF14" s="36"/>
+      <c r="AG14" s="35"/>
+      <c r="AM14" s="54"/>
+      <c r="AN14" s="35"/>
+      <c r="AT14" s="58"/>
+      <c r="AU14" s="35"/>
+      <c r="BA14" s="36"/>
+      <c r="BB14" s="35"/>
+      <c r="BC14" s="57"/>
+      <c r="BH14" s="36"/>
     </row>
     <row r="15" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="51" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="25" t="s">
@@ -2188,62 +2077,62 @@
       <c r="D15" s="33">
         <v>0</v>
       </c>
-      <c r="E15" s="35"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="58"/>
-      <c r="H15" s="58"/>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="59"/>
-      <c r="L15" s="60"/>
-      <c r="M15" s="58"/>
-      <c r="N15" s="58"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="59"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="58"/>
-      <c r="U15" s="58"/>
-      <c r="V15" s="58"/>
-      <c r="W15" s="61"/>
-      <c r="X15" s="58"/>
-      <c r="Y15" s="59"/>
-      <c r="Z15" s="60"/>
-      <c r="AA15" s="58"/>
-      <c r="AB15" s="58"/>
-      <c r="AC15" s="58"/>
-      <c r="AD15" s="58"/>
-      <c r="AE15" s="58"/>
-      <c r="AF15" s="59"/>
-      <c r="AG15" s="60"/>
-      <c r="AH15" s="58"/>
-      <c r="AI15" s="58"/>
-      <c r="AJ15" s="58"/>
-      <c r="AK15" s="58"/>
-      <c r="AL15" s="58"/>
-      <c r="AM15" s="59"/>
-      <c r="AN15" s="60"/>
-      <c r="AO15" s="58"/>
-      <c r="AP15" s="58"/>
-      <c r="AQ15" s="58"/>
-      <c r="AR15" s="58"/>
-      <c r="AS15" s="58"/>
-      <c r="AT15" s="72"/>
-      <c r="AU15" s="60"/>
-      <c r="AV15" s="58"/>
-      <c r="AW15" s="58"/>
-      <c r="AX15" s="58"/>
-      <c r="AY15" s="58"/>
-      <c r="AZ15" s="58"/>
-      <c r="BA15" s="59"/>
-      <c r="BB15" s="60"/>
-      <c r="BC15" s="71"/>
-      <c r="BD15" s="58"/>
-      <c r="BE15" s="58"/>
-      <c r="BF15" s="58"/>
-      <c r="BG15" s="58"/>
-      <c r="BH15" s="59"/>
+      <c r="E15" s="51"/>
+      <c r="F15" s="51"/>
+      <c r="G15" s="51"/>
+      <c r="H15" s="51"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="51"/>
+      <c r="K15" s="51"/>
+      <c r="L15" s="51"/>
+      <c r="M15" s="51"/>
+      <c r="N15" s="51"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="51"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
+      <c r="Y15" s="51"/>
+      <c r="Z15" s="51"/>
+      <c r="AA15" s="51"/>
+      <c r="AB15" s="51"/>
+      <c r="AC15" s="51"/>
+      <c r="AD15" s="51"/>
+      <c r="AE15" s="51"/>
+      <c r="AF15" s="51"/>
+      <c r="AG15" s="51"/>
+      <c r="AH15" s="51"/>
+      <c r="AI15" s="51"/>
+      <c r="AJ15" s="51"/>
+      <c r="AK15" s="51"/>
+      <c r="AL15" s="51"/>
+      <c r="AM15" s="51"/>
+      <c r="AN15" s="51"/>
+      <c r="AO15" s="51"/>
+      <c r="AP15" s="51"/>
+      <c r="AQ15" s="51"/>
+      <c r="AR15" s="51"/>
+      <c r="AS15" s="51"/>
+      <c r="AT15" s="58"/>
+      <c r="AU15" s="51"/>
+      <c r="AV15" s="51"/>
+      <c r="AW15" s="51"/>
+      <c r="AX15" s="51"/>
+      <c r="AY15" s="51"/>
+      <c r="AZ15" s="51"/>
+      <c r="BA15" s="51"/>
+      <c r="BB15" s="51"/>
+      <c r="BC15" s="57"/>
+      <c r="BD15" s="51"/>
+      <c r="BE15" s="51"/>
+      <c r="BF15" s="51"/>
+      <c r="BG15" s="51"/>
+      <c r="BH15" s="51"/>
     </row>
     <row r="16" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="25" t="s">
@@ -2255,61 +2144,26 @@
         <v>0</v>
       </c>
       <c r="E16" s="35"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="58"/>
-      <c r="K16" s="59"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="58"/>
-      <c r="N16" s="58"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="58"/>
-      <c r="Q16" s="70"/>
-      <c r="R16" s="69"/>
-      <c r="S16" s="69"/>
-      <c r="T16" s="69"/>
-      <c r="U16" s="69"/>
-      <c r="V16" s="69"/>
-      <c r="W16" s="68"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="62"/>
-      <c r="Z16" s="61"/>
-      <c r="AA16" s="58"/>
-      <c r="AB16" s="58"/>
-      <c r="AC16" s="58"/>
-      <c r="AD16" s="58"/>
-      <c r="AE16" s="58"/>
-      <c r="AF16" s="59"/>
-      <c r="AG16" s="60"/>
-      <c r="AH16" s="58"/>
-      <c r="AI16" s="58"/>
-      <c r="AJ16" s="58"/>
-      <c r="AK16" s="58"/>
-      <c r="AL16" s="58"/>
-      <c r="AM16" s="59"/>
-      <c r="AN16" s="60"/>
-      <c r="AO16" s="58"/>
-      <c r="AP16" s="58"/>
-      <c r="AQ16" s="58"/>
-      <c r="AR16" s="58"/>
-      <c r="AS16" s="58"/>
-      <c r="AT16" s="72"/>
-      <c r="AU16" s="60"/>
-      <c r="AV16" s="58"/>
-      <c r="AW16" s="58"/>
-      <c r="AX16" s="58"/>
-      <c r="AY16" s="58"/>
-      <c r="AZ16" s="58"/>
-      <c r="BA16" s="59"/>
-      <c r="BB16" s="60"/>
-      <c r="BC16" s="71"/>
-      <c r="BD16" s="58"/>
-      <c r="BE16" s="58"/>
-      <c r="BF16" s="58"/>
-      <c r="BG16" s="58"/>
-      <c r="BH16" s="59"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="35"/>
+      <c r="Q16" s="56"/>
+      <c r="R16" s="55"/>
+      <c r="S16" s="55"/>
+      <c r="T16" s="55"/>
+      <c r="U16" s="55"/>
+      <c r="V16" s="55"/>
+      <c r="W16" s="54"/>
+      <c r="Y16" s="48"/>
+      <c r="AF16" s="36"/>
+      <c r="AG16" s="35"/>
+      <c r="AM16" s="36"/>
+      <c r="AN16" s="35"/>
+      <c r="AT16" s="58"/>
+      <c r="AU16" s="35"/>
+      <c r="BA16" s="36"/>
+      <c r="BB16" s="35"/>
+      <c r="BC16" s="57"/>
+      <c r="BH16" s="36"/>
     </row>
     <row r="17" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="25" t="s">
@@ -2321,61 +2175,28 @@
         <v>0</v>
       </c>
       <c r="E17" s="35"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="58"/>
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
-      <c r="J17" s="58"/>
-      <c r="K17" s="59"/>
-      <c r="L17" s="60"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
-      <c r="O17" s="61"/>
-      <c r="P17" s="58"/>
-      <c r="Q17" s="69"/>
-      <c r="R17" s="69"/>
-      <c r="S17" s="69"/>
-      <c r="T17" s="69"/>
-      <c r="U17" s="69"/>
-      <c r="V17" s="69"/>
-      <c r="W17" s="69"/>
-      <c r="X17" s="69"/>
-      <c r="Y17" s="68"/>
-      <c r="Z17" s="60"/>
-      <c r="AA17" s="58"/>
-      <c r="AB17" s="58"/>
-      <c r="AC17" s="58"/>
-      <c r="AD17" s="58"/>
-      <c r="AE17" s="58"/>
-      <c r="AF17" s="59"/>
-      <c r="AG17" s="60"/>
-      <c r="AH17" s="58"/>
-      <c r="AI17" s="58"/>
-      <c r="AJ17" s="58"/>
-      <c r="AK17" s="58"/>
-      <c r="AL17" s="58"/>
-      <c r="AM17" s="59"/>
-      <c r="AN17" s="60"/>
-      <c r="AO17" s="58"/>
-      <c r="AP17" s="58"/>
-      <c r="AQ17" s="58"/>
-      <c r="AR17" s="58"/>
-      <c r="AS17" s="58"/>
-      <c r="AT17" s="72"/>
-      <c r="AU17" s="60"/>
-      <c r="AV17" s="58"/>
-      <c r="AW17" s="58"/>
-      <c r="AX17" s="58"/>
-      <c r="AY17" s="58"/>
-      <c r="AZ17" s="58"/>
-      <c r="BA17" s="59"/>
-      <c r="BB17" s="60"/>
-      <c r="BC17" s="71"/>
-      <c r="BD17" s="58"/>
-      <c r="BE17" s="58"/>
-      <c r="BF17" s="58"/>
-      <c r="BG17" s="58"/>
-      <c r="BH17" s="59"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="35"/>
+      <c r="Q17" s="55"/>
+      <c r="R17" s="55"/>
+      <c r="S17" s="55"/>
+      <c r="T17" s="55"/>
+      <c r="U17" s="55"/>
+      <c r="V17" s="55"/>
+      <c r="W17" s="55"/>
+      <c r="X17" s="55"/>
+      <c r="Y17" s="54"/>
+      <c r="Z17" s="35"/>
+      <c r="AF17" s="36"/>
+      <c r="AG17" s="35"/>
+      <c r="AM17" s="36"/>
+      <c r="AN17" s="35"/>
+      <c r="AT17" s="58"/>
+      <c r="AU17" s="35"/>
+      <c r="BA17" s="36"/>
+      <c r="BB17" s="35"/>
+      <c r="BC17" s="57"/>
+      <c r="BH17" s="36"/>
     </row>
     <row r="18" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="25" t="s">
@@ -2387,64 +2208,31 @@
         <v>0</v>
       </c>
       <c r="E18" s="35"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
-      <c r="J18" s="58"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="60"/>
-      <c r="M18" s="58"/>
-      <c r="N18" s="58"/>
-      <c r="O18" s="61"/>
-      <c r="P18" s="58"/>
-      <c r="Q18" s="69"/>
-      <c r="R18" s="69"/>
-      <c r="S18" s="69"/>
-      <c r="T18" s="69"/>
-      <c r="U18" s="69"/>
-      <c r="V18" s="69"/>
-      <c r="W18" s="69"/>
-      <c r="X18" s="69"/>
-      <c r="Y18" s="68"/>
-      <c r="Z18" s="60"/>
-      <c r="AA18" s="58"/>
-      <c r="AB18" s="58"/>
-      <c r="AC18" s="58"/>
-      <c r="AD18" s="58"/>
-      <c r="AE18" s="58"/>
-      <c r="AF18" s="59"/>
-      <c r="AG18" s="60"/>
-      <c r="AH18" s="58"/>
-      <c r="AI18" s="58"/>
-      <c r="AJ18" s="58"/>
-      <c r="AK18" s="58"/>
-      <c r="AL18" s="58"/>
-      <c r="AM18" s="59"/>
-      <c r="AN18" s="60"/>
-      <c r="AO18" s="58"/>
-      <c r="AP18" s="58"/>
-      <c r="AQ18" s="58"/>
-      <c r="AR18" s="58"/>
-      <c r="AS18" s="58"/>
-      <c r="AT18" s="72"/>
-      <c r="AU18" s="60"/>
-      <c r="AV18" s="58"/>
-      <c r="AW18" s="58"/>
-      <c r="AX18" s="58"/>
-      <c r="AY18" s="58"/>
-      <c r="AZ18" s="58"/>
-      <c r="BA18" s="59"/>
-      <c r="BB18" s="60"/>
-      <c r="BC18" s="71"/>
-      <c r="BD18" s="58"/>
-      <c r="BE18" s="58"/>
-      <c r="BF18" s="58"/>
-      <c r="BG18" s="58"/>
-      <c r="BH18" s="59"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="35"/>
+      <c r="Q18" s="55"/>
+      <c r="R18" s="55"/>
+      <c r="S18" s="55"/>
+      <c r="T18" s="55"/>
+      <c r="U18" s="55"/>
+      <c r="V18" s="55"/>
+      <c r="W18" s="55"/>
+      <c r="X18" s="55"/>
+      <c r="Y18" s="54"/>
+      <c r="Z18" s="35"/>
+      <c r="AF18" s="36"/>
+      <c r="AG18" s="35"/>
+      <c r="AM18" s="36"/>
+      <c r="AN18" s="35"/>
+      <c r="AT18" s="58"/>
+      <c r="AU18" s="35"/>
+      <c r="BA18" s="36"/>
+      <c r="BB18" s="35"/>
+      <c r="BC18" s="57"/>
+      <c r="BH18" s="36"/>
     </row>
     <row r="19" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="65" t="s">
+      <c r="A19" s="51" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="25" t="s">
@@ -2456,62 +2244,62 @@
       <c r="D19" s="33">
         <v>0</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="58"/>
-      <c r="K19" s="59"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="58"/>
-      <c r="O19" s="58"/>
-      <c r="P19" s="58"/>
-      <c r="Q19" s="58"/>
-      <c r="R19" s="59"/>
-      <c r="S19" s="60"/>
-      <c r="T19" s="58"/>
-      <c r="U19" s="58"/>
-      <c r="V19" s="58"/>
-      <c r="W19" s="58"/>
-      <c r="X19" s="58"/>
-      <c r="Y19" s="59"/>
-      <c r="Z19" s="60"/>
-      <c r="AA19" s="58"/>
-      <c r="AB19" s="58"/>
-      <c r="AC19" s="58"/>
-      <c r="AD19" s="58"/>
-      <c r="AE19" s="58"/>
-      <c r="AF19" s="59"/>
-      <c r="AG19" s="60"/>
-      <c r="AH19" s="58"/>
-      <c r="AI19" s="58"/>
-      <c r="AJ19" s="58"/>
-      <c r="AK19" s="58"/>
-      <c r="AL19" s="58"/>
-      <c r="AM19" s="59"/>
-      <c r="AN19" s="60"/>
-      <c r="AO19" s="58"/>
-      <c r="AP19" s="58"/>
-      <c r="AQ19" s="58"/>
-      <c r="AR19" s="58"/>
-      <c r="AS19" s="58"/>
-      <c r="AT19" s="72"/>
-      <c r="AU19" s="60"/>
-      <c r="AV19" s="58"/>
-      <c r="AW19" s="58"/>
-      <c r="AX19" s="58"/>
-      <c r="AY19" s="58"/>
-      <c r="AZ19" s="58"/>
-      <c r="BA19" s="59"/>
-      <c r="BB19" s="60"/>
-      <c r="BC19" s="71"/>
-      <c r="BD19" s="58"/>
-      <c r="BE19" s="58"/>
-      <c r="BF19" s="58"/>
-      <c r="BG19" s="58"/>
-      <c r="BH19" s="59"/>
+      <c r="E19" s="51"/>
+      <c r="F19" s="51"/>
+      <c r="G19" s="51"/>
+      <c r="H19" s="51"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="51"/>
+      <c r="K19" s="51"/>
+      <c r="L19" s="51"/>
+      <c r="M19" s="51"/>
+      <c r="N19" s="51"/>
+      <c r="O19" s="51"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="51"/>
+      <c r="R19" s="51"/>
+      <c r="S19" s="51"/>
+      <c r="T19" s="51"/>
+      <c r="U19" s="51"/>
+      <c r="V19" s="51"/>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="51"/>
+      <c r="AB19" s="51"/>
+      <c r="AC19" s="51"/>
+      <c r="AD19" s="51"/>
+      <c r="AE19" s="51"/>
+      <c r="AF19" s="51"/>
+      <c r="AG19" s="51"/>
+      <c r="AH19" s="51"/>
+      <c r="AI19" s="51"/>
+      <c r="AJ19" s="51"/>
+      <c r="AK19" s="51"/>
+      <c r="AL19" s="51"/>
+      <c r="AM19" s="51"/>
+      <c r="AN19" s="51"/>
+      <c r="AO19" s="51"/>
+      <c r="AP19" s="51"/>
+      <c r="AQ19" s="51"/>
+      <c r="AR19" s="51"/>
+      <c r="AS19" s="51"/>
+      <c r="AT19" s="58"/>
+      <c r="AU19" s="51"/>
+      <c r="AV19" s="51"/>
+      <c r="AW19" s="51"/>
+      <c r="AX19" s="51"/>
+      <c r="AY19" s="51"/>
+      <c r="AZ19" s="51"/>
+      <c r="BA19" s="51"/>
+      <c r="BB19" s="51"/>
+      <c r="BC19" s="57"/>
+      <c r="BD19" s="51"/>
+      <c r="BE19" s="51"/>
+      <c r="BF19" s="51"/>
+      <c r="BG19" s="51"/>
+      <c r="BH19" s="51"/>
     </row>
     <row r="20" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="25" t="s">
@@ -2523,61 +2311,23 @@
         <v>0</v>
       </c>
       <c r="E20" s="35"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="68"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
-      <c r="K20" s="59"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="58"/>
-      <c r="N20" s="58"/>
-      <c r="O20" s="58"/>
-      <c r="P20" s="58"/>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="59"/>
-      <c r="S20" s="60"/>
-      <c r="T20" s="58"/>
-      <c r="U20" s="58"/>
-      <c r="V20" s="58"/>
-      <c r="W20" s="58"/>
-      <c r="X20" s="58"/>
-      <c r="Y20" s="59"/>
-      <c r="Z20" s="60"/>
-      <c r="AA20" s="58"/>
-      <c r="AB20" s="58"/>
-      <c r="AC20" s="58"/>
-      <c r="AD20" s="58"/>
-      <c r="AE20" s="58"/>
-      <c r="AF20" s="59"/>
-      <c r="AG20" s="60"/>
-      <c r="AH20" s="58"/>
-      <c r="AI20" s="58"/>
-      <c r="AJ20" s="58"/>
-      <c r="AK20" s="58"/>
-      <c r="AL20" s="58"/>
-      <c r="AM20" s="59"/>
-      <c r="AN20" s="60"/>
-      <c r="AO20" s="58"/>
-      <c r="AP20" s="58"/>
-      <c r="AQ20" s="58"/>
-      <c r="AR20" s="58"/>
-      <c r="AS20" s="58"/>
-      <c r="AT20" s="72"/>
-      <c r="AU20" s="60"/>
-      <c r="AV20" s="58"/>
-      <c r="AW20" s="58"/>
-      <c r="AX20" s="58"/>
-      <c r="AY20" s="58"/>
-      <c r="AZ20" s="58"/>
-      <c r="BA20" s="59"/>
-      <c r="BB20" s="60"/>
-      <c r="BC20" s="71"/>
-      <c r="BD20" s="58"/>
-      <c r="BE20" s="58"/>
-      <c r="BF20" s="58"/>
-      <c r="BG20" s="58"/>
-      <c r="BH20" s="59"/>
+      <c r="H20" s="54"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="35"/>
+      <c r="R20" s="36"/>
+      <c r="S20" s="35"/>
+      <c r="Y20" s="36"/>
+      <c r="Z20" s="35"/>
+      <c r="AF20" s="36"/>
+      <c r="AG20" s="35"/>
+      <c r="AM20" s="36"/>
+      <c r="AN20" s="35"/>
+      <c r="AT20" s="58"/>
+      <c r="AU20" s="35"/>
+      <c r="BA20" s="36"/>
+      <c r="BB20" s="35"/>
+      <c r="BC20" s="57"/>
+      <c r="BH20" s="36"/>
     </row>
     <row r="21" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="25" t="s">
@@ -2589,61 +2339,24 @@
         <v>0</v>
       </c>
       <c r="E21" s="35"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="58"/>
-      <c r="J21" s="58"/>
-      <c r="K21" s="59"/>
-      <c r="L21" s="60"/>
-      <c r="M21" s="58"/>
-      <c r="N21" s="58"/>
-      <c r="O21" s="58"/>
-      <c r="P21" s="58"/>
-      <c r="Q21" s="58"/>
-      <c r="R21" s="59"/>
-      <c r="S21" s="60"/>
-      <c r="T21" s="58"/>
-      <c r="U21" s="58"/>
-      <c r="V21" s="58"/>
-      <c r="W21" s="58"/>
-      <c r="X21" s="70"/>
-      <c r="Y21" s="70"/>
-      <c r="Z21" s="60"/>
-      <c r="AA21" s="58"/>
-      <c r="AB21" s="58"/>
-      <c r="AC21" s="58"/>
-      <c r="AD21" s="58"/>
-      <c r="AE21" s="58"/>
-      <c r="AF21" s="59"/>
-      <c r="AG21" s="60"/>
-      <c r="AH21" s="58"/>
-      <c r="AI21" s="58"/>
-      <c r="AJ21" s="58"/>
-      <c r="AK21" s="58"/>
-      <c r="AL21" s="58"/>
-      <c r="AM21" s="59"/>
-      <c r="AN21" s="60"/>
-      <c r="AO21" s="58"/>
-      <c r="AP21" s="58"/>
-      <c r="AQ21" s="58"/>
-      <c r="AR21" s="58"/>
-      <c r="AS21" s="58"/>
-      <c r="AT21" s="72"/>
-      <c r="AU21" s="60"/>
-      <c r="AV21" s="58"/>
-      <c r="AW21" s="58"/>
-      <c r="AX21" s="58"/>
-      <c r="AY21" s="58"/>
-      <c r="AZ21" s="58"/>
-      <c r="BA21" s="59"/>
-      <c r="BB21" s="60"/>
-      <c r="BC21" s="71"/>
-      <c r="BD21" s="58"/>
-      <c r="BE21" s="58"/>
-      <c r="BF21" s="58"/>
-      <c r="BG21" s="58"/>
-      <c r="BH21" s="59"/>
+      <c r="H21" s="56"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="35"/>
+      <c r="R21" s="36"/>
+      <c r="S21" s="35"/>
+      <c r="X21" s="56"/>
+      <c r="Y21" s="56"/>
+      <c r="Z21" s="35"/>
+      <c r="AF21" s="36"/>
+      <c r="AG21" s="35"/>
+      <c r="AM21" s="36"/>
+      <c r="AN21" s="35"/>
+      <c r="AT21" s="58"/>
+      <c r="AU21" s="35"/>
+      <c r="BA21" s="36"/>
+      <c r="BB21" s="35"/>
+      <c r="BC21" s="57"/>
+      <c r="BH21" s="36"/>
     </row>
     <row r="22" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
@@ -2655,64 +2368,31 @@
         <v>0</v>
       </c>
       <c r="E22" s="35"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="59"/>
-      <c r="L22" s="60"/>
-      <c r="M22" s="58"/>
-      <c r="N22" s="58"/>
-      <c r="O22" s="58"/>
-      <c r="P22" s="58"/>
-      <c r="Q22" s="58"/>
-      <c r="R22" s="59"/>
-      <c r="S22" s="69"/>
-      <c r="T22" s="69"/>
-      <c r="U22" s="69"/>
-      <c r="V22" s="69"/>
-      <c r="W22" s="69"/>
-      <c r="X22" s="69"/>
-      <c r="Y22" s="68"/>
-      <c r="Z22" s="60"/>
-      <c r="AA22" s="58"/>
-      <c r="AB22" s="58"/>
-      <c r="AC22" s="58"/>
-      <c r="AD22" s="58"/>
-      <c r="AE22" s="58"/>
-      <c r="AF22" s="59"/>
-      <c r="AG22" s="60"/>
-      <c r="AH22" s="58"/>
-      <c r="AI22" s="58"/>
-      <c r="AJ22" s="58"/>
-      <c r="AK22" s="58"/>
-      <c r="AL22" s="58"/>
-      <c r="AM22" s="59"/>
-      <c r="AN22" s="60"/>
-      <c r="AO22" s="58"/>
-      <c r="AP22" s="58"/>
-      <c r="AQ22" s="58"/>
-      <c r="AR22" s="58"/>
-      <c r="AS22" s="58"/>
-      <c r="AT22" s="72"/>
-      <c r="AU22" s="60"/>
-      <c r="AV22" s="58"/>
-      <c r="AW22" s="58"/>
-      <c r="AX22" s="58"/>
-      <c r="AY22" s="58"/>
-      <c r="AZ22" s="58"/>
-      <c r="BA22" s="59"/>
-      <c r="BB22" s="60"/>
-      <c r="BC22" s="71"/>
-      <c r="BD22" s="58"/>
-      <c r="BE22" s="58"/>
-      <c r="BF22" s="58"/>
-      <c r="BG22" s="58"/>
-      <c r="BH22" s="59"/>
+      <c r="H22" s="56"/>
+      <c r="K22" s="36"/>
+      <c r="L22" s="35"/>
+      <c r="R22" s="36"/>
+      <c r="S22" s="55"/>
+      <c r="T22" s="55"/>
+      <c r="U22" s="55"/>
+      <c r="V22" s="55"/>
+      <c r="W22" s="55"/>
+      <c r="X22" s="55"/>
+      <c r="Y22" s="54"/>
+      <c r="Z22" s="35"/>
+      <c r="AF22" s="36"/>
+      <c r="AG22" s="35"/>
+      <c r="AM22" s="36"/>
+      <c r="AN22" s="35"/>
+      <c r="AT22" s="58"/>
+      <c r="AU22" s="35"/>
+      <c r="BA22" s="36"/>
+      <c r="BB22" s="35"/>
+      <c r="BC22" s="57"/>
+      <c r="BH22" s="36"/>
     </row>
     <row r="23" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="51" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="25" t="s">
@@ -2722,62 +2402,62 @@
       <c r="D23" s="33">
         <v>0</v>
       </c>
-      <c r="E23" s="35"/>
-      <c r="F23" s="58"/>
-      <c r="G23" s="58"/>
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
-      <c r="J23" s="58"/>
-      <c r="K23" s="59"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="58"/>
-      <c r="N23" s="58"/>
-      <c r="O23" s="58"/>
-      <c r="P23" s="58"/>
-      <c r="Q23" s="58"/>
-      <c r="R23" s="59"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="58"/>
-      <c r="U23" s="58"/>
-      <c r="V23" s="58"/>
-      <c r="W23" s="58"/>
-      <c r="X23" s="58"/>
-      <c r="Y23" s="59"/>
-      <c r="Z23" s="60"/>
-      <c r="AA23" s="58"/>
-      <c r="AB23" s="58"/>
-      <c r="AC23" s="58"/>
-      <c r="AD23" s="58"/>
-      <c r="AE23" s="58"/>
-      <c r="AF23" s="59"/>
-      <c r="AG23" s="60"/>
-      <c r="AH23" s="58"/>
-      <c r="AI23" s="58"/>
-      <c r="AJ23" s="58"/>
-      <c r="AK23" s="58"/>
-      <c r="AL23" s="58"/>
-      <c r="AM23" s="59"/>
-      <c r="AN23" s="60"/>
-      <c r="AO23" s="58"/>
-      <c r="AP23" s="58"/>
-      <c r="AQ23" s="58"/>
-      <c r="AR23" s="58"/>
-      <c r="AS23" s="58"/>
-      <c r="AT23" s="72"/>
-      <c r="AU23" s="60"/>
-      <c r="AV23" s="58"/>
-      <c r="AW23" s="58"/>
-      <c r="AX23" s="58"/>
-      <c r="AY23" s="58"/>
-      <c r="AZ23" s="58"/>
-      <c r="BA23" s="59"/>
-      <c r="BB23" s="60"/>
-      <c r="BC23" s="71"/>
-      <c r="BD23" s="58"/>
-      <c r="BE23" s="58"/>
-      <c r="BF23" s="58"/>
-      <c r="BG23" s="58"/>
-      <c r="BH23" s="59"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
+      <c r="S23" s="51"/>
+      <c r="T23" s="51"/>
+      <c r="U23" s="51"/>
+      <c r="V23" s="51"/>
+      <c r="W23" s="51"/>
+      <c r="X23" s="51"/>
+      <c r="Y23" s="51"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="51"/>
+      <c r="AB23" s="51"/>
+      <c r="AC23" s="51"/>
+      <c r="AD23" s="51"/>
+      <c r="AE23" s="51"/>
+      <c r="AF23" s="51"/>
+      <c r="AG23" s="51"/>
+      <c r="AH23" s="51"/>
+      <c r="AI23" s="51"/>
+      <c r="AJ23" s="51"/>
+      <c r="AK23" s="51"/>
+      <c r="AL23" s="51"/>
+      <c r="AM23" s="51"/>
+      <c r="AN23" s="51"/>
+      <c r="AO23" s="51"/>
+      <c r="AP23" s="51"/>
+      <c r="AQ23" s="51"/>
+      <c r="AR23" s="51"/>
+      <c r="AS23" s="51"/>
+      <c r="AT23" s="58"/>
+      <c r="AU23" s="51"/>
+      <c r="AV23" s="51"/>
+      <c r="AW23" s="51"/>
+      <c r="AX23" s="51"/>
+      <c r="AY23" s="51"/>
+      <c r="AZ23" s="51"/>
+      <c r="BA23" s="51"/>
+      <c r="BB23" s="51"/>
+      <c r="BC23" s="57"/>
+      <c r="BD23" s="51"/>
+      <c r="BE23" s="51"/>
+      <c r="BF23" s="51"/>
+      <c r="BG23" s="51"/>
+      <c r="BH23" s="51"/>
     </row>
     <row r="24" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
@@ -2789,61 +2469,22 @@
         <v>0</v>
       </c>
       <c r="E24" s="35"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="58"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="58"/>
-      <c r="N24" s="58"/>
-      <c r="O24" s="58"/>
-      <c r="P24" s="58"/>
-      <c r="Q24" s="58"/>
-      <c r="R24" s="59"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="58"/>
-      <c r="U24" s="58"/>
-      <c r="V24" s="58"/>
-      <c r="W24" s="58"/>
-      <c r="X24" s="58"/>
-      <c r="Y24" s="59"/>
-      <c r="Z24" s="60"/>
-      <c r="AA24" s="58"/>
-      <c r="AB24" s="58"/>
-      <c r="AC24" s="58"/>
-      <c r="AD24" s="58"/>
-      <c r="AE24" s="58"/>
-      <c r="AF24" s="59"/>
-      <c r="AG24" s="60"/>
-      <c r="AH24" s="58"/>
-      <c r="AI24" s="58"/>
-      <c r="AJ24" s="58"/>
-      <c r="AK24" s="58"/>
-      <c r="AL24" s="58"/>
-      <c r="AM24" s="68"/>
-      <c r="AN24" s="60"/>
-      <c r="AO24" s="58"/>
-      <c r="AP24" s="58"/>
-      <c r="AQ24" s="58"/>
-      <c r="AR24" s="58"/>
-      <c r="AS24" s="58"/>
-      <c r="AT24" s="72"/>
-      <c r="AU24" s="60"/>
-      <c r="AV24" s="58"/>
-      <c r="AW24" s="58"/>
-      <c r="AX24" s="58"/>
-      <c r="AY24" s="58"/>
-      <c r="AZ24" s="58"/>
-      <c r="BA24" s="59"/>
-      <c r="BB24" s="60"/>
-      <c r="BC24" s="71"/>
-      <c r="BD24" s="58"/>
-      <c r="BE24" s="58"/>
-      <c r="BF24" s="58"/>
-      <c r="BG24" s="58"/>
-      <c r="BH24" s="59"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="35"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="35"/>
+      <c r="Y24" s="36"/>
+      <c r="Z24" s="35"/>
+      <c r="AF24" s="36"/>
+      <c r="AG24" s="35"/>
+      <c r="AM24" s="54"/>
+      <c r="AN24" s="35"/>
+      <c r="AT24" s="58"/>
+      <c r="AU24" s="35"/>
+      <c r="BA24" s="36"/>
+      <c r="BB24" s="35"/>
+      <c r="BC24" s="57"/>
+      <c r="BH24" s="36"/>
     </row>
     <row r="25" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
@@ -2855,61 +2496,22 @@
         <v>0</v>
       </c>
       <c r="E25" s="35"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
-      <c r="J25" s="58"/>
-      <c r="K25" s="59"/>
-      <c r="L25" s="60"/>
-      <c r="M25" s="58"/>
-      <c r="N25" s="58"/>
-      <c r="O25" s="58"/>
-      <c r="P25" s="58"/>
-      <c r="Q25" s="58"/>
-      <c r="R25" s="59"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="58"/>
-      <c r="U25" s="58"/>
-      <c r="V25" s="58"/>
-      <c r="W25" s="58"/>
-      <c r="X25" s="58"/>
-      <c r="Y25" s="59"/>
-      <c r="Z25" s="60"/>
-      <c r="AA25" s="58"/>
-      <c r="AB25" s="58"/>
-      <c r="AC25" s="58"/>
-      <c r="AD25" s="58"/>
-      <c r="AE25" s="58"/>
-      <c r="AF25" s="59"/>
-      <c r="AG25" s="60"/>
-      <c r="AH25" s="58"/>
-      <c r="AI25" s="58"/>
-      <c r="AJ25" s="58"/>
-      <c r="AK25" s="58"/>
-      <c r="AL25" s="58"/>
-      <c r="AM25" s="68"/>
-      <c r="AN25" s="60"/>
-      <c r="AO25" s="58"/>
-      <c r="AP25" s="58"/>
-      <c r="AQ25" s="58"/>
-      <c r="AR25" s="58"/>
-      <c r="AS25" s="58"/>
-      <c r="AT25" s="72"/>
-      <c r="AU25" s="60"/>
-      <c r="AV25" s="58"/>
-      <c r="AW25" s="58"/>
-      <c r="AX25" s="58"/>
-      <c r="AY25" s="58"/>
-      <c r="AZ25" s="58"/>
-      <c r="BA25" s="59"/>
-      <c r="BB25" s="60"/>
-      <c r="BC25" s="71"/>
-      <c r="BD25" s="58"/>
-      <c r="BE25" s="58"/>
-      <c r="BF25" s="58"/>
-      <c r="BG25" s="58"/>
-      <c r="BH25" s="59"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="35"/>
+      <c r="R25" s="36"/>
+      <c r="S25" s="35"/>
+      <c r="Y25" s="36"/>
+      <c r="Z25" s="35"/>
+      <c r="AF25" s="36"/>
+      <c r="AG25" s="35"/>
+      <c r="AM25" s="54"/>
+      <c r="AN25" s="35"/>
+      <c r="AT25" s="58"/>
+      <c r="AU25" s="35"/>
+      <c r="BA25" s="36"/>
+      <c r="BB25" s="35"/>
+      <c r="BC25" s="57"/>
+      <c r="BH25" s="36"/>
     </row>
     <row r="26" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
@@ -2921,64 +2523,25 @@
         <v>0</v>
       </c>
       <c r="E26" s="35"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="58"/>
-      <c r="N26" s="58"/>
-      <c r="O26" s="58"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="59"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="58"/>
-      <c r="U26" s="58"/>
-      <c r="V26" s="58"/>
-      <c r="W26" s="58"/>
-      <c r="X26" s="58"/>
-      <c r="Y26" s="59"/>
-      <c r="Z26" s="60"/>
-      <c r="AA26" s="58"/>
-      <c r="AB26" s="58"/>
-      <c r="AC26" s="58"/>
-      <c r="AD26" s="58"/>
-      <c r="AE26" s="58"/>
-      <c r="AF26" s="59"/>
-      <c r="AG26" s="60"/>
-      <c r="AH26" s="58"/>
-      <c r="AI26" s="58"/>
-      <c r="AJ26" s="58"/>
-      <c r="AK26" s="58"/>
-      <c r="AL26" s="58"/>
-      <c r="AM26" s="68"/>
-      <c r="AN26" s="60"/>
-      <c r="AO26" s="58"/>
-      <c r="AP26" s="58"/>
-      <c r="AQ26" s="58"/>
-      <c r="AR26" s="58"/>
-      <c r="AS26" s="58"/>
-      <c r="AT26" s="72"/>
-      <c r="AU26" s="60"/>
-      <c r="AV26" s="58"/>
-      <c r="AW26" s="58"/>
-      <c r="AX26" s="58"/>
-      <c r="AY26" s="58"/>
-      <c r="AZ26" s="58"/>
-      <c r="BA26" s="59"/>
-      <c r="BB26" s="60"/>
-      <c r="BC26" s="71"/>
-      <c r="BD26" s="58"/>
-      <c r="BE26" s="58"/>
-      <c r="BF26" s="58"/>
-      <c r="BG26" s="58"/>
-      <c r="BH26" s="59"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="35"/>
+      <c r="R26" s="36"/>
+      <c r="S26" s="35"/>
+      <c r="Y26" s="36"/>
+      <c r="Z26" s="35"/>
+      <c r="AF26" s="36"/>
+      <c r="AG26" s="35"/>
+      <c r="AM26" s="54"/>
+      <c r="AN26" s="35"/>
+      <c r="AT26" s="58"/>
+      <c r="AU26" s="35"/>
+      <c r="BA26" s="36"/>
+      <c r="BB26" s="35"/>
+      <c r="BC26" s="57"/>
+      <c r="BH26" s="36"/>
     </row>
     <row r="27" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="51" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="25"/>
@@ -2986,62 +2549,62 @@
       <c r="D27" s="33">
         <v>0</v>
       </c>
-      <c r="E27" s="35"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
-      <c r="J27" s="58"/>
-      <c r="K27" s="59"/>
-      <c r="L27" s="60"/>
-      <c r="M27" s="58"/>
-      <c r="N27" s="58"/>
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="59"/>
-      <c r="S27" s="60"/>
-      <c r="T27" s="58"/>
-      <c r="U27" s="58"/>
-      <c r="V27" s="58"/>
-      <c r="W27" s="58"/>
-      <c r="X27" s="58"/>
-      <c r="Y27" s="59"/>
-      <c r="Z27" s="60"/>
-      <c r="AA27" s="58"/>
-      <c r="AB27" s="58"/>
-      <c r="AC27" s="58"/>
-      <c r="AD27" s="58"/>
-      <c r="AE27" s="58"/>
-      <c r="AF27" s="59"/>
-      <c r="AG27" s="60"/>
-      <c r="AH27" s="58"/>
-      <c r="AI27" s="58"/>
-      <c r="AJ27" s="58"/>
-      <c r="AK27" s="58"/>
-      <c r="AL27" s="58"/>
-      <c r="AM27" s="59"/>
-      <c r="AN27" s="60"/>
-      <c r="AO27" s="58"/>
-      <c r="AP27" s="58"/>
-      <c r="AQ27" s="58"/>
-      <c r="AR27" s="58"/>
-      <c r="AS27" s="58"/>
-      <c r="AT27" s="72"/>
-      <c r="AU27" s="60"/>
-      <c r="AV27" s="58"/>
-      <c r="AW27" s="58"/>
-      <c r="AX27" s="58"/>
-      <c r="AY27" s="58"/>
-      <c r="AZ27" s="58"/>
-      <c r="BA27" s="59"/>
-      <c r="BB27" s="60"/>
-      <c r="BC27" s="71"/>
-      <c r="BD27" s="58"/>
-      <c r="BE27" s="58"/>
-      <c r="BF27" s="58"/>
-      <c r="BG27" s="58"/>
-      <c r="BH27" s="59"/>
+      <c r="E27" s="51"/>
+      <c r="F27" s="51"/>
+      <c r="G27" s="51"/>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="51"/>
+      <c r="M27" s="51"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="51"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="51"/>
+      <c r="R27" s="51"/>
+      <c r="S27" s="51"/>
+      <c r="T27" s="51"/>
+      <c r="U27" s="51"/>
+      <c r="V27" s="51"/>
+      <c r="W27" s="51"/>
+      <c r="X27" s="51"/>
+      <c r="Y27" s="51"/>
+      <c r="Z27" s="51"/>
+      <c r="AA27" s="51"/>
+      <c r="AB27" s="51"/>
+      <c r="AC27" s="51"/>
+      <c r="AD27" s="51"/>
+      <c r="AE27" s="51"/>
+      <c r="AF27" s="51"/>
+      <c r="AG27" s="51"/>
+      <c r="AH27" s="51"/>
+      <c r="AI27" s="51"/>
+      <c r="AJ27" s="51"/>
+      <c r="AK27" s="51"/>
+      <c r="AL27" s="51"/>
+      <c r="AM27" s="51"/>
+      <c r="AN27" s="51"/>
+      <c r="AO27" s="51"/>
+      <c r="AP27" s="51"/>
+      <c r="AQ27" s="51"/>
+      <c r="AR27" s="51"/>
+      <c r="AS27" s="51"/>
+      <c r="AT27" s="58"/>
+      <c r="AU27" s="51"/>
+      <c r="AV27" s="51"/>
+      <c r="AW27" s="51"/>
+      <c r="AX27" s="51"/>
+      <c r="AY27" s="51"/>
+      <c r="AZ27" s="51"/>
+      <c r="BA27" s="51"/>
+      <c r="BB27" s="51"/>
+      <c r="BC27" s="57"/>
+      <c r="BD27" s="51"/>
+      <c r="BE27" s="51"/>
+      <c r="BF27" s="51"/>
+      <c r="BG27" s="51"/>
+      <c r="BH27" s="51"/>
     </row>
     <row r="28" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="41" t="s">
@@ -3053,61 +2616,17 @@
         <v>0</v>
       </c>
       <c r="E28" s="35"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="58"/>
-      <c r="N28" s="58"/>
-      <c r="O28" s="58"/>
-      <c r="P28" s="58"/>
-      <c r="Q28" s="58"/>
-      <c r="R28" s="59"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="58"/>
-      <c r="U28" s="58"/>
-      <c r="V28" s="58"/>
-      <c r="W28" s="58"/>
-      <c r="X28" s="58"/>
-      <c r="Y28" s="59"/>
-      <c r="Z28" s="60"/>
-      <c r="AA28" s="58"/>
-      <c r="AB28" s="58"/>
-      <c r="AC28" s="58"/>
-      <c r="AD28" s="58"/>
-      <c r="AE28" s="58"/>
-      <c r="AF28" s="59"/>
-      <c r="AG28" s="61"/>
-      <c r="AH28" s="58"/>
-      <c r="AI28" s="58"/>
-      <c r="AJ28" s="58"/>
-      <c r="AK28" s="58"/>
-      <c r="AL28" s="58"/>
-      <c r="AM28" s="61"/>
-      <c r="AN28" s="61"/>
-      <c r="AO28" s="58"/>
-      <c r="AP28" s="58"/>
-      <c r="AQ28" s="58"/>
-      <c r="AR28" s="58"/>
-      <c r="AS28" s="58"/>
-      <c r="AT28" s="72"/>
-      <c r="AU28" s="61"/>
-      <c r="AV28" s="58"/>
-      <c r="AW28" s="58"/>
-      <c r="AX28" s="58"/>
-      <c r="AY28" s="58"/>
-      <c r="AZ28" s="58"/>
-      <c r="BA28" s="61"/>
-      <c r="BB28" s="60"/>
-      <c r="BC28" s="71"/>
-      <c r="BD28" s="58"/>
-      <c r="BE28" s="58"/>
-      <c r="BF28" s="58"/>
-      <c r="BG28" s="58"/>
-      <c r="BH28" s="59"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="35"/>
+      <c r="R28" s="36"/>
+      <c r="S28" s="35"/>
+      <c r="Y28" s="36"/>
+      <c r="Z28" s="35"/>
+      <c r="AF28" s="36"/>
+      <c r="AT28" s="58"/>
+      <c r="BB28" s="35"/>
+      <c r="BC28" s="57"/>
+      <c r="BH28" s="36"/>
     </row>
     <row r="29" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="41" t="s">
@@ -3119,64 +2638,20 @@
         <v>0</v>
       </c>
       <c r="E29" s="35"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
-      <c r="J29" s="58"/>
-      <c r="K29" s="59"/>
-      <c r="L29" s="60"/>
-      <c r="M29" s="58"/>
-      <c r="N29" s="58"/>
-      <c r="O29" s="58"/>
-      <c r="P29" s="58"/>
-      <c r="Q29" s="58"/>
-      <c r="R29" s="59"/>
-      <c r="S29" s="60"/>
-      <c r="T29" s="58"/>
-      <c r="U29" s="58"/>
-      <c r="V29" s="58"/>
-      <c r="W29" s="58"/>
-      <c r="X29" s="58"/>
-      <c r="Y29" s="59"/>
-      <c r="Z29" s="60"/>
-      <c r="AA29" s="58"/>
-      <c r="AB29" s="58"/>
-      <c r="AC29" s="58"/>
-      <c r="AD29" s="58"/>
-      <c r="AE29" s="58"/>
-      <c r="AF29" s="59"/>
-      <c r="AG29" s="61"/>
-      <c r="AH29" s="58"/>
-      <c r="AI29" s="58"/>
-      <c r="AJ29" s="58"/>
-      <c r="AK29" s="58"/>
-      <c r="AL29" s="58"/>
-      <c r="AM29" s="61"/>
-      <c r="AN29" s="61"/>
-      <c r="AO29" s="58"/>
-      <c r="AP29" s="58"/>
-      <c r="AQ29" s="58"/>
-      <c r="AR29" s="58"/>
-      <c r="AS29" s="58"/>
-      <c r="AT29" s="72"/>
-      <c r="AU29" s="61"/>
-      <c r="AV29" s="58"/>
-      <c r="AW29" s="58"/>
-      <c r="AX29" s="58"/>
-      <c r="AY29" s="58"/>
-      <c r="AZ29" s="58"/>
-      <c r="BA29" s="61"/>
-      <c r="BB29" s="60"/>
-      <c r="BC29" s="71"/>
-      <c r="BD29" s="58"/>
-      <c r="BE29" s="58"/>
-      <c r="BF29" s="58"/>
-      <c r="BG29" s="58"/>
-      <c r="BH29" s="59"/>
+      <c r="K29" s="36"/>
+      <c r="L29" s="35"/>
+      <c r="R29" s="36"/>
+      <c r="S29" s="35"/>
+      <c r="Y29" s="36"/>
+      <c r="Z29" s="35"/>
+      <c r="AF29" s="36"/>
+      <c r="AT29" s="58"/>
+      <c r="BB29" s="35"/>
+      <c r="BC29" s="57"/>
+      <c r="BH29" s="36"/>
     </row>
     <row r="30" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="52" t="s">
         <v>34</v>
       </c>
       <c r="B30" s="25"/>
@@ -3184,62 +2659,62 @@
       <c r="D30" s="33">
         <v>0</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
-      <c r="J30" s="58"/>
-      <c r="K30" s="59"/>
-      <c r="L30" s="60"/>
-      <c r="M30" s="58"/>
-      <c r="N30" s="58"/>
-      <c r="O30" s="58"/>
-      <c r="P30" s="58"/>
-      <c r="Q30" s="58"/>
-      <c r="R30" s="59"/>
-      <c r="S30" s="60"/>
-      <c r="T30" s="58"/>
-      <c r="U30" s="58"/>
-      <c r="V30" s="58"/>
-      <c r="W30" s="58"/>
-      <c r="X30" s="58"/>
-      <c r="Y30" s="59"/>
-      <c r="Z30" s="60"/>
-      <c r="AA30" s="58"/>
-      <c r="AB30" s="58"/>
-      <c r="AC30" s="58"/>
-      <c r="AD30" s="58"/>
-      <c r="AE30" s="58"/>
-      <c r="AF30" s="59"/>
-      <c r="AG30" s="58"/>
-      <c r="AH30" s="58"/>
-      <c r="AI30" s="58"/>
-      <c r="AJ30" s="58"/>
-      <c r="AK30" s="58"/>
-      <c r="AL30" s="58"/>
-      <c r="AM30" s="62"/>
-      <c r="AN30" s="58"/>
-      <c r="AO30" s="58"/>
-      <c r="AP30" s="58"/>
-      <c r="AQ30" s="58"/>
-      <c r="AR30" s="58"/>
-      <c r="AS30" s="58"/>
-      <c r="AT30" s="72"/>
-      <c r="AU30" s="58"/>
-      <c r="AV30" s="58"/>
-      <c r="AW30" s="58"/>
-      <c r="AX30" s="58"/>
-      <c r="AY30" s="58"/>
-      <c r="AZ30" s="58"/>
-      <c r="BA30" s="58"/>
-      <c r="BB30" s="60"/>
-      <c r="BC30" s="71"/>
-      <c r="BD30" s="58"/>
-      <c r="BE30" s="58"/>
-      <c r="BF30" s="58"/>
-      <c r="BG30" s="58"/>
-      <c r="BH30" s="59"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="51"/>
+      <c r="M30" s="51"/>
+      <c r="N30" s="51"/>
+      <c r="O30" s="51"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="51"/>
+      <c r="R30" s="51"/>
+      <c r="S30" s="51"/>
+      <c r="T30" s="51"/>
+      <c r="U30" s="51"/>
+      <c r="V30" s="51"/>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
+      <c r="Y30" s="51"/>
+      <c r="Z30" s="51"/>
+      <c r="AA30" s="51"/>
+      <c r="AB30" s="51"/>
+      <c r="AC30" s="51"/>
+      <c r="AD30" s="51"/>
+      <c r="AE30" s="51"/>
+      <c r="AF30" s="51"/>
+      <c r="AG30" s="51"/>
+      <c r="AH30" s="51"/>
+      <c r="AI30" s="51"/>
+      <c r="AJ30" s="51"/>
+      <c r="AK30" s="51"/>
+      <c r="AL30" s="51"/>
+      <c r="AM30" s="51"/>
+      <c r="AN30" s="51"/>
+      <c r="AO30" s="51"/>
+      <c r="AP30" s="51"/>
+      <c r="AQ30" s="51"/>
+      <c r="AR30" s="51"/>
+      <c r="AS30" s="51"/>
+      <c r="AT30" s="58"/>
+      <c r="AU30" s="51"/>
+      <c r="AV30" s="51"/>
+      <c r="AW30" s="51"/>
+      <c r="AX30" s="51"/>
+      <c r="AY30" s="51"/>
+      <c r="AZ30" s="51"/>
+      <c r="BA30" s="51"/>
+      <c r="BB30" s="51"/>
+      <c r="BC30" s="57"/>
+      <c r="BD30" s="51"/>
+      <c r="BE30" s="51"/>
+      <c r="BF30" s="51"/>
+      <c r="BG30" s="51"/>
+      <c r="BH30" s="51"/>
     </row>
     <row r="31" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="41" t="s">
@@ -3251,61 +2726,17 @@
         <v>0</v>
       </c>
       <c r="E31" s="35"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
-      <c r="J31" s="58"/>
-      <c r="K31" s="59"/>
-      <c r="L31" s="60"/>
-      <c r="M31" s="58"/>
-      <c r="N31" s="58"/>
-      <c r="O31" s="58"/>
-      <c r="P31" s="58"/>
-      <c r="Q31" s="58"/>
-      <c r="R31" s="59"/>
-      <c r="S31" s="60"/>
-      <c r="T31" s="58"/>
-      <c r="U31" s="58"/>
-      <c r="V31" s="58"/>
-      <c r="W31" s="58"/>
-      <c r="X31" s="58"/>
-      <c r="Y31" s="59"/>
-      <c r="Z31" s="60"/>
-      <c r="AA31" s="58"/>
-      <c r="AB31" s="58"/>
-      <c r="AC31" s="58"/>
-      <c r="AD31" s="58"/>
-      <c r="AE31" s="58"/>
-      <c r="AF31" s="59"/>
-      <c r="AG31" s="58"/>
-      <c r="AH31" s="58"/>
-      <c r="AI31" s="58"/>
-      <c r="AJ31" s="58"/>
-      <c r="AK31" s="58"/>
-      <c r="AL31" s="58"/>
-      <c r="AM31" s="61"/>
-      <c r="AN31" s="58"/>
-      <c r="AO31" s="58"/>
-      <c r="AP31" s="58"/>
-      <c r="AQ31" s="58"/>
-      <c r="AR31" s="58"/>
-      <c r="AS31" s="58"/>
-      <c r="AT31" s="72"/>
-      <c r="AU31" s="58"/>
-      <c r="AV31" s="58"/>
-      <c r="AW31" s="58"/>
-      <c r="AX31" s="58"/>
-      <c r="AY31" s="58"/>
-      <c r="AZ31" s="58"/>
-      <c r="BA31" s="58"/>
-      <c r="BB31" s="60"/>
-      <c r="BC31" s="71"/>
-      <c r="BD31" s="58"/>
-      <c r="BE31" s="58"/>
-      <c r="BF31" s="58"/>
-      <c r="BG31" s="58"/>
-      <c r="BH31" s="59"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="35"/>
+      <c r="R31" s="36"/>
+      <c r="S31" s="35"/>
+      <c r="Y31" s="36"/>
+      <c r="Z31" s="35"/>
+      <c r="AF31" s="36"/>
+      <c r="AT31" s="58"/>
+      <c r="BB31" s="35"/>
+      <c r="BC31" s="57"/>
+      <c r="BH31" s="36"/>
     </row>
     <row r="32" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="41" t="s">
@@ -3317,61 +2748,17 @@
         <v>0</v>
       </c>
       <c r="E32" s="35"/>
-      <c r="F32" s="58"/>
-      <c r="G32" s="58"/>
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
-      <c r="J32" s="58"/>
-      <c r="K32" s="59"/>
-      <c r="L32" s="60"/>
-      <c r="M32" s="58"/>
-      <c r="N32" s="58"/>
-      <c r="O32" s="58"/>
-      <c r="P32" s="58"/>
-      <c r="Q32" s="58"/>
-      <c r="R32" s="59"/>
-      <c r="S32" s="60"/>
-      <c r="T32" s="58"/>
-      <c r="U32" s="58"/>
-      <c r="V32" s="58"/>
-      <c r="W32" s="58"/>
-      <c r="X32" s="58"/>
-      <c r="Y32" s="59"/>
-      <c r="Z32" s="60"/>
-      <c r="AA32" s="58"/>
-      <c r="AB32" s="58"/>
-      <c r="AC32" s="58"/>
-      <c r="AD32" s="58"/>
-      <c r="AE32" s="58"/>
-      <c r="AF32" s="59"/>
-      <c r="AG32" s="58"/>
-      <c r="AH32" s="58"/>
-      <c r="AI32" s="58"/>
-      <c r="AJ32" s="58"/>
-      <c r="AK32" s="58"/>
-      <c r="AL32" s="58"/>
-      <c r="AM32" s="61"/>
-      <c r="AN32" s="58"/>
-      <c r="AO32" s="58"/>
-      <c r="AP32" s="58"/>
-      <c r="AQ32" s="58"/>
-      <c r="AR32" s="58"/>
-      <c r="AS32" s="58"/>
-      <c r="AT32" s="72"/>
-      <c r="AU32" s="58"/>
-      <c r="AV32" s="58"/>
-      <c r="AW32" s="58"/>
-      <c r="AX32" s="58"/>
-      <c r="AY32" s="58"/>
-      <c r="AZ32" s="58"/>
-      <c r="BA32" s="58"/>
-      <c r="BB32" s="60"/>
-      <c r="BC32" s="71"/>
-      <c r="BD32" s="58"/>
-      <c r="BE32" s="58"/>
-      <c r="BF32" s="58"/>
-      <c r="BG32" s="58"/>
-      <c r="BH32" s="59"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="35"/>
+      <c r="R32" s="36"/>
+      <c r="S32" s="35"/>
+      <c r="Y32" s="36"/>
+      <c r="Z32" s="35"/>
+      <c r="AF32" s="36"/>
+      <c r="AT32" s="58"/>
+      <c r="BB32" s="35"/>
+      <c r="BC32" s="57"/>
+      <c r="BH32" s="36"/>
     </row>
     <row r="33" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="41" t="s">
@@ -3383,61 +2770,17 @@
         <v>0</v>
       </c>
       <c r="E33" s="35"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
-      <c r="J33" s="58"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="58"/>
-      <c r="N33" s="58"/>
-      <c r="O33" s="58"/>
-      <c r="P33" s="58"/>
-      <c r="Q33" s="58"/>
-      <c r="R33" s="59"/>
-      <c r="S33" s="60"/>
-      <c r="T33" s="58"/>
-      <c r="U33" s="58"/>
-      <c r="V33" s="58"/>
-      <c r="W33" s="58"/>
-      <c r="X33" s="58"/>
-      <c r="Y33" s="59"/>
-      <c r="Z33" s="60"/>
-      <c r="AA33" s="58"/>
-      <c r="AB33" s="58"/>
-      <c r="AC33" s="58"/>
-      <c r="AD33" s="58"/>
-      <c r="AE33" s="58"/>
-      <c r="AF33" s="59"/>
-      <c r="AG33" s="58"/>
-      <c r="AH33" s="58"/>
-      <c r="AI33" s="58"/>
-      <c r="AJ33" s="58"/>
-      <c r="AK33" s="58"/>
-      <c r="AL33" s="58"/>
-      <c r="AM33" s="61"/>
-      <c r="AN33" s="58"/>
-      <c r="AO33" s="58"/>
-      <c r="AP33" s="58"/>
-      <c r="AQ33" s="58"/>
-      <c r="AR33" s="58"/>
-      <c r="AS33" s="58"/>
-      <c r="AT33" s="72"/>
-      <c r="AU33" s="58"/>
-      <c r="AV33" s="58"/>
-      <c r="AW33" s="58"/>
-      <c r="AX33" s="58"/>
-      <c r="AY33" s="58"/>
-      <c r="AZ33" s="58"/>
-      <c r="BA33" s="58"/>
-      <c r="BB33" s="60"/>
-      <c r="BC33" s="71"/>
-      <c r="BD33" s="58"/>
-      <c r="BE33" s="58"/>
-      <c r="BF33" s="58"/>
-      <c r="BG33" s="58"/>
-      <c r="BH33" s="59"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="35"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="35"/>
+      <c r="Y33" s="36"/>
+      <c r="Z33" s="35"/>
+      <c r="AF33" s="36"/>
+      <c r="AT33" s="58"/>
+      <c r="BB33" s="35"/>
+      <c r="BC33" s="57"/>
+      <c r="BH33" s="36"/>
     </row>
     <row r="34" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="41" t="s">
@@ -3449,64 +2792,20 @@
         <v>0</v>
       </c>
       <c r="E34" s="35"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="59"/>
-      <c r="S34" s="60"/>
-      <c r="T34" s="58"/>
-      <c r="U34" s="58"/>
-      <c r="V34" s="58"/>
-      <c r="W34" s="58"/>
-      <c r="X34" s="58"/>
-      <c r="Y34" s="59"/>
-      <c r="Z34" s="60"/>
-      <c r="AA34" s="58"/>
-      <c r="AB34" s="58"/>
-      <c r="AC34" s="58"/>
-      <c r="AD34" s="58"/>
-      <c r="AE34" s="58"/>
-      <c r="AF34" s="59"/>
-      <c r="AG34" s="58"/>
-      <c r="AH34" s="58"/>
-      <c r="AI34" s="58"/>
-      <c r="AJ34" s="58"/>
-      <c r="AK34" s="58"/>
-      <c r="AL34" s="58"/>
-      <c r="AM34" s="61"/>
-      <c r="AN34" s="58"/>
-      <c r="AO34" s="58"/>
-      <c r="AP34" s="58"/>
-      <c r="AQ34" s="58"/>
-      <c r="AR34" s="58"/>
-      <c r="AS34" s="58"/>
-      <c r="AT34" s="72"/>
-      <c r="AU34" s="58"/>
-      <c r="AV34" s="58"/>
-      <c r="AW34" s="58"/>
-      <c r="AX34" s="58"/>
-      <c r="AY34" s="58"/>
-      <c r="AZ34" s="58"/>
-      <c r="BA34" s="58"/>
-      <c r="BB34" s="60"/>
-      <c r="BC34" s="71"/>
-      <c r="BD34" s="58"/>
-      <c r="BE34" s="58"/>
-      <c r="BF34" s="58"/>
-      <c r="BG34" s="58"/>
-      <c r="BH34" s="59"/>
+      <c r="K34" s="36"/>
+      <c r="L34" s="35"/>
+      <c r="R34" s="36"/>
+      <c r="S34" s="35"/>
+      <c r="Y34" s="36"/>
+      <c r="Z34" s="35"/>
+      <c r="AF34" s="36"/>
+      <c r="AT34" s="58"/>
+      <c r="BB34" s="35"/>
+      <c r="BC34" s="57"/>
+      <c r="BH34" s="36"/>
     </row>
     <row r="35" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="65" t="s">
+      <c r="A35" s="51" t="s">
         <v>35</v>
       </c>
       <c r="B35" s="25"/>
@@ -3514,62 +2813,62 @@
       <c r="D35" s="33">
         <v>0</v>
       </c>
-      <c r="E35" s="35"/>
-      <c r="F35" s="58"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
-      <c r="J35" s="58"/>
-      <c r="K35" s="59"/>
-      <c r="L35" s="60"/>
-      <c r="M35" s="58"/>
-      <c r="N35" s="58"/>
-      <c r="O35" s="58"/>
-      <c r="P35" s="58"/>
-      <c r="Q35" s="58"/>
-      <c r="R35" s="59"/>
-      <c r="S35" s="60"/>
-      <c r="T35" s="58"/>
-      <c r="U35" s="58"/>
-      <c r="V35" s="58"/>
-      <c r="W35" s="58"/>
-      <c r="X35" s="58"/>
-      <c r="Y35" s="59"/>
-      <c r="Z35" s="60"/>
-      <c r="AA35" s="58"/>
-      <c r="AB35" s="58"/>
-      <c r="AC35" s="58"/>
-      <c r="AD35" s="58"/>
-      <c r="AE35" s="58"/>
-      <c r="AF35" s="59"/>
-      <c r="AG35" s="60"/>
-      <c r="AH35" s="58"/>
-      <c r="AI35" s="58"/>
-      <c r="AJ35" s="58"/>
-      <c r="AK35" s="58"/>
-      <c r="AL35" s="58"/>
-      <c r="AM35" s="59"/>
-      <c r="AN35" s="60"/>
-      <c r="AO35" s="58"/>
-      <c r="AP35" s="58"/>
-      <c r="AQ35" s="58"/>
-      <c r="AR35" s="58"/>
-      <c r="AS35" s="58"/>
-      <c r="AT35" s="72"/>
-      <c r="AU35" s="60"/>
-      <c r="AV35" s="58"/>
-      <c r="AW35" s="58"/>
-      <c r="AX35" s="58"/>
-      <c r="AY35" s="58"/>
-      <c r="AZ35" s="58"/>
-      <c r="BA35" s="59"/>
-      <c r="BB35" s="60"/>
-      <c r="BC35" s="71"/>
-      <c r="BD35" s="58"/>
-      <c r="BE35" s="58"/>
-      <c r="BF35" s="58"/>
-      <c r="BG35" s="58"/>
-      <c r="BH35" s="59"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="51"/>
+      <c r="H35" s="51"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="51"/>
+      <c r="M35" s="51"/>
+      <c r="N35" s="51"/>
+      <c r="O35" s="51"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="51"/>
+      <c r="R35" s="51"/>
+      <c r="S35" s="51"/>
+      <c r="T35" s="51"/>
+      <c r="U35" s="51"/>
+      <c r="V35" s="51"/>
+      <c r="W35" s="51"/>
+      <c r="X35" s="51"/>
+      <c r="Y35" s="51"/>
+      <c r="Z35" s="51"/>
+      <c r="AA35" s="51"/>
+      <c r="AB35" s="51"/>
+      <c r="AC35" s="51"/>
+      <c r="AD35" s="51"/>
+      <c r="AE35" s="51"/>
+      <c r="AF35" s="51"/>
+      <c r="AG35" s="51"/>
+      <c r="AH35" s="51"/>
+      <c r="AI35" s="51"/>
+      <c r="AJ35" s="51"/>
+      <c r="AK35" s="51"/>
+      <c r="AL35" s="51"/>
+      <c r="AM35" s="51"/>
+      <c r="AN35" s="51"/>
+      <c r="AO35" s="51"/>
+      <c r="AP35" s="51"/>
+      <c r="AQ35" s="51"/>
+      <c r="AR35" s="51"/>
+      <c r="AS35" s="51"/>
+      <c r="AT35" s="58"/>
+      <c r="AU35" s="51"/>
+      <c r="AV35" s="51"/>
+      <c r="AW35" s="51"/>
+      <c r="AX35" s="51"/>
+      <c r="AY35" s="51"/>
+      <c r="AZ35" s="51"/>
+      <c r="BA35" s="51"/>
+      <c r="BB35" s="51"/>
+      <c r="BC35" s="57"/>
+      <c r="BD35" s="51"/>
+      <c r="BE35" s="51"/>
+      <c r="BF35" s="51"/>
+      <c r="BG35" s="51"/>
+      <c r="BH35" s="51"/>
     </row>
     <row r="36" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="41" t="s">
@@ -3581,61 +2880,27 @@
         <v>0</v>
       </c>
       <c r="E36" s="35"/>
-      <c r="F36" s="58"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="58"/>
-      <c r="N36" s="58"/>
-      <c r="O36" s="58"/>
-      <c r="P36" s="58"/>
-      <c r="Q36" s="58"/>
-      <c r="R36" s="70"/>
-      <c r="S36" s="69"/>
-      <c r="T36" s="69"/>
-      <c r="U36" s="69"/>
-      <c r="V36" s="69"/>
-      <c r="W36" s="69"/>
-      <c r="X36" s="69"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="35"/>
+      <c r="R36" s="56"/>
+      <c r="S36" s="55"/>
+      <c r="T36" s="55"/>
+      <c r="U36" s="55"/>
+      <c r="V36" s="55"/>
+      <c r="W36" s="55"/>
+      <c r="X36" s="55"/>
       <c r="Y36" s="42"/>
-      <c r="Z36" s="60"/>
-      <c r="AA36" s="58"/>
-      <c r="AB36" s="58"/>
-      <c r="AC36" s="58"/>
-      <c r="AD36" s="58"/>
-      <c r="AE36" s="58"/>
-      <c r="AF36" s="59"/>
-      <c r="AG36" s="60"/>
-      <c r="AH36" s="58"/>
-      <c r="AI36" s="58"/>
-      <c r="AJ36" s="58"/>
-      <c r="AK36" s="58"/>
-      <c r="AL36" s="58"/>
-      <c r="AM36" s="59"/>
-      <c r="AN36" s="60"/>
-      <c r="AO36" s="58"/>
-      <c r="AP36" s="58"/>
-      <c r="AQ36" s="58"/>
-      <c r="AR36" s="58"/>
-      <c r="AS36" s="58"/>
-      <c r="AT36" s="72"/>
-      <c r="AU36" s="60"/>
-      <c r="AV36" s="58"/>
-      <c r="AW36" s="58"/>
-      <c r="AX36" s="58"/>
-      <c r="AY36" s="58"/>
-      <c r="AZ36" s="58"/>
-      <c r="BA36" s="59"/>
-      <c r="BB36" s="60"/>
-      <c r="BC36" s="71"/>
-      <c r="BD36" s="58"/>
-      <c r="BE36" s="58"/>
-      <c r="BF36" s="58"/>
-      <c r="BG36" s="58"/>
-      <c r="BH36" s="59"/>
+      <c r="Z36" s="35"/>
+      <c r="AF36" s="36"/>
+      <c r="AG36" s="35"/>
+      <c r="AM36" s="36"/>
+      <c r="AN36" s="35"/>
+      <c r="AT36" s="58"/>
+      <c r="AU36" s="35"/>
+      <c r="BA36" s="36"/>
+      <c r="BB36" s="35"/>
+      <c r="BC36" s="57"/>
+      <c r="BH36" s="36"/>
     </row>
     <row r="37" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="41" t="s">
@@ -3647,61 +2912,22 @@
         <v>0</v>
       </c>
       <c r="E37" s="35"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="58"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="59"/>
-      <c r="S37" s="60"/>
-      <c r="T37" s="58"/>
-      <c r="U37" s="58"/>
-      <c r="V37" s="58"/>
-      <c r="W37" s="58"/>
-      <c r="X37" s="58"/>
-      <c r="Y37" s="59"/>
-      <c r="Z37" s="60"/>
-      <c r="AA37" s="58"/>
-      <c r="AB37" s="58"/>
-      <c r="AC37" s="58"/>
-      <c r="AD37" s="58"/>
-      <c r="AE37" s="58"/>
-      <c r="AF37" s="59"/>
-      <c r="AG37" s="60"/>
-      <c r="AH37" s="58"/>
-      <c r="AI37" s="58"/>
-      <c r="AJ37" s="58"/>
-      <c r="AK37" s="58"/>
-      <c r="AL37" s="58"/>
-      <c r="AM37" s="59"/>
-      <c r="AN37" s="60"/>
-      <c r="AO37" s="58"/>
-      <c r="AP37" s="58"/>
-      <c r="AQ37" s="58"/>
-      <c r="AR37" s="58"/>
-      <c r="AS37" s="58"/>
-      <c r="AT37" s="72"/>
-      <c r="AU37" s="60"/>
-      <c r="AV37" s="58"/>
-      <c r="AW37" s="58"/>
-      <c r="AX37" s="58"/>
-      <c r="AY37" s="58"/>
-      <c r="AZ37" s="58"/>
-      <c r="BA37" s="59"/>
-      <c r="BB37" s="68"/>
-      <c r="BC37" s="71"/>
-      <c r="BD37" s="58"/>
-      <c r="BE37" s="58"/>
-      <c r="BF37" s="58"/>
-      <c r="BG37" s="58"/>
-      <c r="BH37" s="59"/>
+      <c r="K37" s="36"/>
+      <c r="L37" s="35"/>
+      <c r="R37" s="36"/>
+      <c r="S37" s="35"/>
+      <c r="Y37" s="36"/>
+      <c r="Z37" s="35"/>
+      <c r="AF37" s="36"/>
+      <c r="AG37" s="35"/>
+      <c r="AM37" s="36"/>
+      <c r="AN37" s="35"/>
+      <c r="AT37" s="58"/>
+      <c r="AU37" s="35"/>
+      <c r="BA37" s="36"/>
+      <c r="BB37" s="54"/>
+      <c r="BC37" s="57"/>
+      <c r="BH37" s="36"/>
     </row>
     <row r="38" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="41" t="s">
@@ -3713,61 +2939,27 @@
         <v>0</v>
       </c>
       <c r="E38" s="35"/>
-      <c r="F38" s="58"/>
-      <c r="G38" s="58"/>
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
-      <c r="J38" s="58"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="67"/>
-      <c r="M38" s="58"/>
-      <c r="N38" s="58"/>
-      <c r="O38" s="58"/>
-      <c r="P38" s="58"/>
-      <c r="Q38" s="58"/>
-      <c r="R38" s="70"/>
-      <c r="S38" s="69"/>
-      <c r="T38" s="69"/>
-      <c r="U38" s="69"/>
-      <c r="V38" s="69"/>
-      <c r="W38" s="69"/>
-      <c r="X38" s="69"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="53"/>
+      <c r="R38" s="56"/>
+      <c r="S38" s="55"/>
+      <c r="T38" s="55"/>
+      <c r="U38" s="55"/>
+      <c r="V38" s="55"/>
+      <c r="W38" s="55"/>
+      <c r="X38" s="55"/>
       <c r="Y38" s="42"/>
-      <c r="Z38" s="60"/>
-      <c r="AA38" s="58"/>
-      <c r="AB38" s="58"/>
-      <c r="AC38" s="58"/>
-      <c r="AD38" s="58"/>
-      <c r="AE38" s="58"/>
-      <c r="AF38" s="59"/>
-      <c r="AG38" s="60"/>
-      <c r="AH38" s="58"/>
-      <c r="AI38" s="58"/>
-      <c r="AJ38" s="58"/>
-      <c r="AK38" s="58"/>
-      <c r="AL38" s="58"/>
-      <c r="AM38" s="59"/>
-      <c r="AN38" s="60"/>
-      <c r="AO38" s="58"/>
-      <c r="AP38" s="58"/>
-      <c r="AQ38" s="58"/>
-      <c r="AR38" s="58"/>
-      <c r="AS38" s="58"/>
-      <c r="AT38" s="72"/>
-      <c r="AU38" s="60"/>
-      <c r="AV38" s="58"/>
-      <c r="AW38" s="58"/>
-      <c r="AX38" s="58"/>
-      <c r="AY38" s="58"/>
-      <c r="AZ38" s="58"/>
-      <c r="BA38" s="59"/>
-      <c r="BB38" s="60"/>
-      <c r="BC38" s="71"/>
-      <c r="BD38" s="58"/>
-      <c r="BE38" s="58"/>
-      <c r="BF38" s="58"/>
-      <c r="BG38" s="58"/>
-      <c r="BH38" s="59"/>
+      <c r="Z38" s="35"/>
+      <c r="AF38" s="36"/>
+      <c r="AG38" s="35"/>
+      <c r="AM38" s="36"/>
+      <c r="AN38" s="35"/>
+      <c r="AT38" s="58"/>
+      <c r="AU38" s="35"/>
+      <c r="BA38" s="36"/>
+      <c r="BB38" s="35"/>
+      <c r="BC38" s="57"/>
+      <c r="BH38" s="36"/>
     </row>
     <row r="39" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
@@ -3779,61 +2971,22 @@
         <v>0</v>
       </c>
       <c r="E39" s="35"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
-      <c r="J39" s="58"/>
-      <c r="K39" s="59"/>
-      <c r="L39" s="60"/>
-      <c r="M39" s="58"/>
-      <c r="N39" s="58"/>
-      <c r="O39" s="58"/>
-      <c r="P39" s="58"/>
-      <c r="Q39" s="58"/>
-      <c r="R39" s="59"/>
-      <c r="S39" s="60"/>
-      <c r="T39" s="58"/>
-      <c r="U39" s="58"/>
-      <c r="V39" s="58"/>
-      <c r="W39" s="58"/>
-      <c r="X39" s="58"/>
-      <c r="Y39" s="59"/>
-      <c r="Z39" s="60"/>
-      <c r="AA39" s="58"/>
-      <c r="AB39" s="58"/>
-      <c r="AC39" s="58"/>
-      <c r="AD39" s="58"/>
-      <c r="AE39" s="58"/>
-      <c r="AF39" s="59"/>
-      <c r="AG39" s="60"/>
-      <c r="AH39" s="58"/>
-      <c r="AI39" s="58"/>
-      <c r="AJ39" s="58"/>
-      <c r="AK39" s="58"/>
-      <c r="AL39" s="58"/>
-      <c r="AM39" s="59"/>
-      <c r="AN39" s="60"/>
-      <c r="AO39" s="58"/>
-      <c r="AP39" s="58"/>
-      <c r="AQ39" s="58"/>
-      <c r="AR39" s="58"/>
-      <c r="AS39" s="58"/>
-      <c r="AT39" s="72"/>
-      <c r="AU39" s="60"/>
-      <c r="AV39" s="58"/>
-      <c r="AW39" s="58"/>
-      <c r="AX39" s="58"/>
-      <c r="AY39" s="58"/>
-      <c r="AZ39" s="58"/>
-      <c r="BA39" s="59"/>
-      <c r="BB39" s="60"/>
-      <c r="BC39" s="71"/>
-      <c r="BD39" s="58"/>
-      <c r="BE39" s="58"/>
-      <c r="BF39" s="58"/>
-      <c r="BG39" s="58"/>
-      <c r="BH39" s="59"/>
+      <c r="K39" s="36"/>
+      <c r="L39" s="35"/>
+      <c r="R39" s="36"/>
+      <c r="S39" s="35"/>
+      <c r="Y39" s="36"/>
+      <c r="Z39" s="35"/>
+      <c r="AF39" s="36"/>
+      <c r="AG39" s="35"/>
+      <c r="AM39" s="36"/>
+      <c r="AN39" s="35"/>
+      <c r="AT39" s="58"/>
+      <c r="AU39" s="35"/>
+      <c r="BA39" s="36"/>
+      <c r="BB39" s="35"/>
+      <c r="BC39" s="57"/>
+      <c r="BH39" s="36"/>
     </row>
     <row r="40" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="41" t="s">
@@ -3845,61 +2998,22 @@
         <v>0</v>
       </c>
       <c r="E40" s="35"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
-      <c r="J40" s="58"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="60"/>
-      <c r="M40" s="58"/>
-      <c r="N40" s="58"/>
-      <c r="O40" s="58"/>
-      <c r="P40" s="58"/>
-      <c r="Q40" s="58"/>
-      <c r="R40" s="59"/>
-      <c r="S40" s="60"/>
-      <c r="T40" s="58"/>
-      <c r="U40" s="58"/>
-      <c r="V40" s="58"/>
-      <c r="W40" s="58"/>
-      <c r="X40" s="58"/>
-      <c r="Y40" s="59"/>
-      <c r="Z40" s="60"/>
-      <c r="AA40" s="58"/>
-      <c r="AB40" s="58"/>
-      <c r="AC40" s="58"/>
-      <c r="AD40" s="58"/>
-      <c r="AE40" s="58"/>
-      <c r="AF40" s="59"/>
-      <c r="AG40" s="60"/>
-      <c r="AH40" s="58"/>
-      <c r="AI40" s="58"/>
-      <c r="AJ40" s="58"/>
-      <c r="AK40" s="58"/>
-      <c r="AL40" s="58"/>
-      <c r="AM40" s="59"/>
-      <c r="AN40" s="60"/>
-      <c r="AO40" s="58"/>
-      <c r="AP40" s="58"/>
-      <c r="AQ40" s="58"/>
-      <c r="AR40" s="58"/>
-      <c r="AS40" s="58"/>
-      <c r="AT40" s="72"/>
-      <c r="AU40" s="60"/>
-      <c r="AV40" s="58"/>
-      <c r="AW40" s="58"/>
-      <c r="AX40" s="58"/>
-      <c r="AY40" s="58"/>
-      <c r="AZ40" s="58"/>
-      <c r="BA40" s="59"/>
-      <c r="BB40" s="60"/>
-      <c r="BC40" s="71"/>
-      <c r="BD40" s="58"/>
-      <c r="BE40" s="58"/>
-      <c r="BF40" s="58"/>
-      <c r="BG40" s="58"/>
-      <c r="BH40" s="59"/>
+      <c r="K40" s="36"/>
+      <c r="L40" s="35"/>
+      <c r="R40" s="36"/>
+      <c r="S40" s="35"/>
+      <c r="Y40" s="36"/>
+      <c r="Z40" s="35"/>
+      <c r="AF40" s="36"/>
+      <c r="AG40" s="35"/>
+      <c r="AM40" s="36"/>
+      <c r="AN40" s="35"/>
+      <c r="AT40" s="58"/>
+      <c r="AU40" s="35"/>
+      <c r="BA40" s="36"/>
+      <c r="BB40" s="35"/>
+      <c r="BC40" s="57"/>
+      <c r="BH40" s="36"/>
     </row>
     <row r="41" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="41" t="s">
@@ -3911,64 +3025,25 @@
         <v>0</v>
       </c>
       <c r="E41" s="35"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="59"/>
-      <c r="L41" s="60"/>
-      <c r="M41" s="58"/>
-      <c r="N41" s="58"/>
-      <c r="O41" s="58"/>
-      <c r="P41" s="58"/>
-      <c r="Q41" s="58"/>
-      <c r="R41" s="59"/>
-      <c r="S41" s="60"/>
-      <c r="T41" s="58"/>
-      <c r="U41" s="58"/>
-      <c r="V41" s="58"/>
-      <c r="W41" s="58"/>
-      <c r="X41" s="58"/>
-      <c r="Y41" s="59"/>
-      <c r="Z41" s="60"/>
-      <c r="AA41" s="58"/>
-      <c r="AB41" s="58"/>
-      <c r="AC41" s="58"/>
-      <c r="AD41" s="58"/>
-      <c r="AE41" s="58"/>
-      <c r="AF41" s="59"/>
-      <c r="AG41" s="60"/>
-      <c r="AH41" s="58"/>
-      <c r="AI41" s="58"/>
-      <c r="AJ41" s="58"/>
-      <c r="AK41" s="58"/>
-      <c r="AL41" s="58"/>
-      <c r="AM41" s="59"/>
-      <c r="AN41" s="60"/>
-      <c r="AO41" s="58"/>
-      <c r="AP41" s="58"/>
-      <c r="AQ41" s="58"/>
-      <c r="AR41" s="58"/>
-      <c r="AS41" s="58"/>
-      <c r="AT41" s="72"/>
-      <c r="AU41" s="60"/>
-      <c r="AV41" s="58"/>
-      <c r="AW41" s="58"/>
-      <c r="AX41" s="58"/>
-      <c r="AY41" s="58"/>
-      <c r="AZ41" s="58"/>
-      <c r="BA41" s="59"/>
-      <c r="BB41" s="60"/>
-      <c r="BC41" s="71"/>
-      <c r="BD41" s="58"/>
-      <c r="BE41" s="58"/>
-      <c r="BF41" s="58"/>
-      <c r="BG41" s="58"/>
-      <c r="BH41" s="59"/>
+      <c r="K41" s="36"/>
+      <c r="L41" s="35"/>
+      <c r="R41" s="36"/>
+      <c r="S41" s="35"/>
+      <c r="Y41" s="36"/>
+      <c r="Z41" s="35"/>
+      <c r="AF41" s="36"/>
+      <c r="AG41" s="35"/>
+      <c r="AM41" s="36"/>
+      <c r="AN41" s="35"/>
+      <c r="AT41" s="58"/>
+      <c r="AU41" s="35"/>
+      <c r="BA41" s="36"/>
+      <c r="BB41" s="35"/>
+      <c r="BC41" s="57"/>
+      <c r="BH41" s="36"/>
     </row>
     <row r="42" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="52" t="s">
         <v>36</v>
       </c>
       <c r="B42" s="25"/>
@@ -3976,62 +3051,62 @@
       <c r="D42" s="33">
         <v>0</v>
       </c>
-      <c r="E42" s="35"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
-      <c r="J42" s="58"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="60"/>
-      <c r="M42" s="58"/>
-      <c r="N42" s="58"/>
-      <c r="O42" s="58"/>
-      <c r="P42" s="58"/>
-      <c r="Q42" s="58"/>
-      <c r="R42" s="59"/>
-      <c r="S42" s="60"/>
-      <c r="T42" s="58"/>
-      <c r="U42" s="58"/>
-      <c r="V42" s="58"/>
-      <c r="W42" s="58"/>
-      <c r="X42" s="58"/>
-      <c r="Y42" s="59"/>
-      <c r="Z42" s="60"/>
-      <c r="AA42" s="58"/>
-      <c r="AB42" s="58"/>
-      <c r="AC42" s="58"/>
-      <c r="AD42" s="58"/>
-      <c r="AE42" s="58"/>
-      <c r="AF42" s="59"/>
-      <c r="AG42" s="60"/>
-      <c r="AH42" s="58"/>
-      <c r="AI42" s="58"/>
-      <c r="AJ42" s="58"/>
-      <c r="AK42" s="58"/>
-      <c r="AL42" s="58"/>
-      <c r="AM42" s="59"/>
-      <c r="AN42" s="60"/>
-      <c r="AO42" s="58"/>
-      <c r="AP42" s="58"/>
-      <c r="AQ42" s="58"/>
-      <c r="AR42" s="58"/>
-      <c r="AS42" s="58"/>
-      <c r="AT42" s="72"/>
-      <c r="AU42" s="60"/>
-      <c r="AV42" s="58"/>
-      <c r="AW42" s="58"/>
-      <c r="AX42" s="58"/>
-      <c r="AY42" s="58"/>
-      <c r="AZ42" s="58"/>
-      <c r="BA42" s="59"/>
-      <c r="BB42" s="60"/>
-      <c r="BC42" s="71"/>
-      <c r="BD42" s="58"/>
-      <c r="BE42" s="58"/>
-      <c r="BF42" s="58"/>
-      <c r="BG42" s="58"/>
-      <c r="BH42" s="59"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="51"/>
+      <c r="H42" s="51"/>
+      <c r="I42" s="51"/>
+      <c r="J42" s="51"/>
+      <c r="K42" s="51"/>
+      <c r="L42" s="51"/>
+      <c r="M42" s="51"/>
+      <c r="N42" s="51"/>
+      <c r="O42" s="51"/>
+      <c r="P42" s="51"/>
+      <c r="Q42" s="51"/>
+      <c r="R42" s="51"/>
+      <c r="S42" s="51"/>
+      <c r="T42" s="51"/>
+      <c r="U42" s="51"/>
+      <c r="V42" s="51"/>
+      <c r="W42" s="51"/>
+      <c r="X42" s="51"/>
+      <c r="Y42" s="51"/>
+      <c r="Z42" s="51"/>
+      <c r="AA42" s="51"/>
+      <c r="AB42" s="51"/>
+      <c r="AC42" s="51"/>
+      <c r="AD42" s="51"/>
+      <c r="AE42" s="51"/>
+      <c r="AF42" s="51"/>
+      <c r="AG42" s="51"/>
+      <c r="AH42" s="51"/>
+      <c r="AI42" s="51"/>
+      <c r="AJ42" s="51"/>
+      <c r="AK42" s="51"/>
+      <c r="AL42" s="51"/>
+      <c r="AM42" s="51"/>
+      <c r="AN42" s="51"/>
+      <c r="AO42" s="51"/>
+      <c r="AP42" s="51"/>
+      <c r="AQ42" s="51"/>
+      <c r="AR42" s="51"/>
+      <c r="AS42" s="51"/>
+      <c r="AT42" s="58"/>
+      <c r="AU42" s="51"/>
+      <c r="AV42" s="51"/>
+      <c r="AW42" s="51"/>
+      <c r="AX42" s="51"/>
+      <c r="AY42" s="51"/>
+      <c r="AZ42" s="51"/>
+      <c r="BA42" s="51"/>
+      <c r="BB42" s="51"/>
+      <c r="BC42" s="57"/>
+      <c r="BD42" s="51"/>
+      <c r="BE42" s="51"/>
+      <c r="BF42" s="51"/>
+      <c r="BG42" s="51"/>
+      <c r="BH42" s="51"/>
     </row>
     <row r="43" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="25" t="s">
@@ -4043,61 +3118,27 @@
         <v>0</v>
       </c>
       <c r="E43" s="35"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
-      <c r="K43" s="59"/>
-      <c r="L43" s="60"/>
-      <c r="M43" s="58"/>
-      <c r="N43" s="58"/>
-      <c r="O43" s="58"/>
-      <c r="P43" s="58"/>
-      <c r="Q43" s="58"/>
-      <c r="R43" s="59"/>
-      <c r="S43" s="60"/>
-      <c r="T43" s="58"/>
-      <c r="U43" s="58"/>
-      <c r="V43" s="58"/>
-      <c r="W43" s="58"/>
-      <c r="X43" s="58"/>
-      <c r="Y43" s="59"/>
-      <c r="Z43" s="60"/>
-      <c r="AA43" s="58"/>
-      <c r="AB43" s="58"/>
-      <c r="AC43" s="58"/>
-      <c r="AD43" s="58"/>
-      <c r="AE43" s="58"/>
-      <c r="AF43" s="59"/>
-      <c r="AG43" s="60"/>
-      <c r="AH43" s="58"/>
-      <c r="AI43" s="58"/>
-      <c r="AJ43" s="58"/>
-      <c r="AK43" s="58"/>
-      <c r="AL43" s="58"/>
-      <c r="AM43" s="59"/>
-      <c r="AN43" s="60"/>
-      <c r="AO43" s="58"/>
-      <c r="AP43" s="58"/>
-      <c r="AQ43" s="58"/>
-      <c r="AR43" s="58"/>
-      <c r="AS43" s="58"/>
-      <c r="AT43" s="72"/>
-      <c r="AU43" s="69"/>
-      <c r="AV43" s="69"/>
-      <c r="AW43" s="69"/>
-      <c r="AX43" s="69"/>
-      <c r="AY43" s="69"/>
-      <c r="AZ43" s="69"/>
-      <c r="BA43" s="69"/>
+      <c r="K43" s="36"/>
+      <c r="L43" s="35"/>
+      <c r="R43" s="36"/>
+      <c r="S43" s="35"/>
+      <c r="Y43" s="36"/>
+      <c r="Z43" s="35"/>
+      <c r="AF43" s="36"/>
+      <c r="AG43" s="35"/>
+      <c r="AM43" s="36"/>
+      <c r="AN43" s="35"/>
+      <c r="AT43" s="58"/>
+      <c r="AU43" s="55"/>
+      <c r="AV43" s="55"/>
+      <c r="AW43" s="55"/>
+      <c r="AX43" s="55"/>
+      <c r="AY43" s="55"/>
+      <c r="AZ43" s="55"/>
+      <c r="BA43" s="55"/>
       <c r="BB43" s="31"/>
-      <c r="BC43" s="58"/>
-      <c r="BD43" s="58"/>
-      <c r="BE43" s="58"/>
-      <c r="BF43" s="58"/>
-      <c r="BG43" s="58"/>
-      <c r="BH43" s="59"/>
+      <c r="BC43" s="57"/>
+      <c r="BH43" s="36"/>
     </row>
     <row r="44" spans="1:60" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="25"/>
@@ -5422,18 +4463,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5575,6 +4616,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B33C0204-9DCF-4E21-BC5C-7978C236823E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4962763A-021A-4368-9A4A-00367974B297}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -5587,14 +4636,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B33C0204-9DCF-4E21-BC5C-7978C236823E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
forgot some thing for the PLANNING
</commit_message>
<xml_diff>
--- a/PLANNING/Task Planning.xlsx
+++ b/PLANNING/Task Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SoftwareProjects\Unity\Band-Battle\PLANNING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16866B8E-DCFF-4E98-B977-2D2DE5F0E15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E50147-2DCE-4512-9713-7A13DF64F1E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{70D4C62D-D84E-421C-8B35-459A60CD8044}"/>
   </bookViews>
@@ -967,6 +967,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="28" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -997,7 +998,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -1326,7 +1326,7 @@
       <pane xSplit="4" ySplit="10" topLeftCell="L11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="AJ13" sqref="AJ13"/>
+      <selection pane="bottomRight" activeCell="AO22" sqref="AO22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1339,69 +1339,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="F1" s="60" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="62"/>
+      <c r="F1" s="61" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="63"/>
     </row>
     <row r="2" spans="1:60" x14ac:dyDescent="0.3">
       <c r="F2" s="32"/>
-      <c r="G2" s="66" t="s">
+      <c r="G2" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="68"/>
     </row>
     <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="F3" s="29"/>
-      <c r="G3" s="66" t="s">
+      <c r="G3" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="68"/>
     </row>
     <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="F4" s="31"/>
-      <c r="G4" s="66" t="s">
+      <c r="G4" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="68"/>
     </row>
     <row r="5" spans="1:60" ht="14.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F5" s="30"/>
-      <c r="G5" s="68" t="s">
+      <c r="G5" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
-      <c r="L5" s="68"/>
-      <c r="M5" s="68"/>
-      <c r="N5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="70"/>
     </row>
     <row r="6" spans="1:60" x14ac:dyDescent="0.3">
       <c r="F6" s="59"/>
@@ -1416,78 +1416,78 @@
       <c r="D7" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="64" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="63" t="s">
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-      <c r="O7" s="64"/>
-      <c r="P7" s="64"/>
-      <c r="Q7" s="64"/>
-      <c r="R7" s="65"/>
-      <c r="S7" s="63" t="s">
+      <c r="M7" s="65"/>
+      <c r="N7" s="65"/>
+      <c r="O7" s="65"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
+      <c r="R7" s="66"/>
+      <c r="S7" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="65"/>
-      <c r="Z7" s="63" t="s">
+      <c r="T7" s="65"/>
+      <c r="U7" s="65"/>
+      <c r="V7" s="65"/>
+      <c r="W7" s="65"/>
+      <c r="X7" s="65"/>
+      <c r="Y7" s="66"/>
+      <c r="Z7" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="AA7" s="64"/>
-      <c r="AB7" s="64"/>
-      <c r="AC7" s="64"/>
-      <c r="AD7" s="64"/>
-      <c r="AE7" s="64"/>
-      <c r="AF7" s="65"/>
-      <c r="AG7" s="63" t="s">
+      <c r="AA7" s="65"/>
+      <c r="AB7" s="65"/>
+      <c r="AC7" s="65"/>
+      <c r="AD7" s="65"/>
+      <c r="AE7" s="65"/>
+      <c r="AF7" s="66"/>
+      <c r="AG7" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="AH7" s="64"/>
-      <c r="AI7" s="64"/>
-      <c r="AJ7" s="64"/>
-      <c r="AK7" s="64"/>
-      <c r="AL7" s="64"/>
-      <c r="AM7" s="65"/>
-      <c r="AN7" s="63" t="s">
+      <c r="AH7" s="65"/>
+      <c r="AI7" s="65"/>
+      <c r="AJ7" s="65"/>
+      <c r="AK7" s="65"/>
+      <c r="AL7" s="65"/>
+      <c r="AM7" s="66"/>
+      <c r="AN7" s="64" t="s">
         <v>9</v>
       </c>
-      <c r="AO7" s="64"/>
-      <c r="AP7" s="64"/>
-      <c r="AQ7" s="64"/>
-      <c r="AR7" s="64"/>
-      <c r="AS7" s="64"/>
-      <c r="AT7" s="65"/>
-      <c r="AU7" s="63" t="s">
+      <c r="AO7" s="65"/>
+      <c r="AP7" s="65"/>
+      <c r="AQ7" s="65"/>
+      <c r="AR7" s="65"/>
+      <c r="AS7" s="65"/>
+      <c r="AT7" s="66"/>
+      <c r="AU7" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="AV7" s="64"/>
-      <c r="AW7" s="64"/>
-      <c r="AX7" s="64"/>
-      <c r="AY7" s="64"/>
-      <c r="AZ7" s="64"/>
-      <c r="BA7" s="65"/>
-      <c r="BB7" s="63" t="s">
+      <c r="AV7" s="65"/>
+      <c r="AW7" s="65"/>
+      <c r="AX7" s="65"/>
+      <c r="AY7" s="65"/>
+      <c r="AZ7" s="65"/>
+      <c r="BA7" s="66"/>
+      <c r="BB7" s="64" t="s">
         <v>11</v>
       </c>
-      <c r="BC7" s="64"/>
-      <c r="BD7" s="64"/>
-      <c r="BE7" s="64"/>
-      <c r="BF7" s="64"/>
-      <c r="BG7" s="64"/>
-      <c r="BH7" s="65"/>
+      <c r="BC7" s="65"/>
+      <c r="BD7" s="65"/>
+      <c r="BE7" s="65"/>
+      <c r="BF7" s="65"/>
+      <c r="BG7" s="65"/>
+      <c r="BH7" s="66"/>
     </row>
     <row r="8" spans="1:60" ht="69.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14"/>
@@ -2055,13 +2055,13 @@
       <c r="W13" s="50"/>
       <c r="Y13" s="49"/>
       <c r="Z13" s="50"/>
-      <c r="AB13" s="70"/>
-      <c r="AC13" s="70"/>
-      <c r="AD13" s="70"/>
-      <c r="AE13" s="70"/>
-      <c r="AF13" s="70"/>
-      <c r="AG13" s="70"/>
-      <c r="AH13" s="70"/>
+      <c r="AB13" s="60"/>
+      <c r="AC13" s="60"/>
+      <c r="AD13" s="60"/>
+      <c r="AE13" s="60"/>
+      <c r="AF13" s="60"/>
+      <c r="AG13" s="60"/>
+      <c r="AH13" s="60"/>
       <c r="AI13" s="55"/>
       <c r="AJ13" s="55"/>
       <c r="AK13" s="55"/>
@@ -2790,6 +2790,13 @@
       <c r="Y31" s="36"/>
       <c r="Z31" s="35"/>
       <c r="AF31" s="36"/>
+      <c r="AI31" s="55"/>
+      <c r="AJ31" s="55"/>
+      <c r="AK31" s="55"/>
+      <c r="AL31" s="55"/>
+      <c r="AM31" s="55"/>
+      <c r="AN31" s="55"/>
+      <c r="AO31" s="54"/>
       <c r="AT31" s="58"/>
       <c r="BB31" s="35"/>
       <c r="BC31" s="57"/>
@@ -4529,18 +4536,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4682,14 +4689,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B33C0204-9DCF-4E21-BC5C-7978C236823E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4962763A-021A-4368-9A4A-00367974B297}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -4702,6 +4701,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B33C0204-9DCF-4E21-BC5C-7978C236823E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>